<commit_message>
Screen and Memory settings translated
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\My Spreadsheets\Amiga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DAB18D-CB6A-4611-8446-5C5B882F1C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091BB30-43ED-4654-A643-E754DE535F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="1665" windowWidth="26175" windowHeight="18015" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="14745" yWindow="2535" windowWidth="36465" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="685">
   <si>
     <t>ID</t>
   </si>
@@ -1687,9 +1687,6 @@
     <t>1.3 ROM, OCS, 512 KB Chip + 512 KB Slow RAM (most common)\nThis configuration is capable of running most games and demos produced for first-generation hardware. Only few exceptions need a different configuration (e.g. the oldest games tend to be incompatible with this configuration).\n1.3 ROM, ECS Agnus, 512 KB Chip RAM + 512 KB Slow RAM\nLater hardware revision of the A500. Nearly 100% compatible with the previous configuration.\n1.3 ROM, ECS Agnus, 1 MB Chip RAM\nFew newer games and demos require this configuration.\n1.3 ROM, OCS Agnus, 512 KB Chip RAM\nVery old (e.g. pre-1988) games and demos may require this configuration.\n1.2 ROM, OCS Agnus, 512 KB Chip RAM\nAs available for the A1000, and installed on the first A500 and A2000 series. Some very old programs only work correctly with this configuration. Note: This system ROM version can only boot from floppy disk (no hard disk boot support).\n1.2 ROM, OCS Agnus, 512 KB Chip RAM + 512 KB Slow RAM\nThis configuration adds expansion memory to the first A500 produced. Try this if your game does not work with newer configurations, but works with the previous one. It could add some features to the game, including faster loading times. Note: This system ROM version can only boot from floppy disk (no hard disk boot support).</t>
   </si>
   <si>
-    <t>Configurazione di base non espansa\nL'A500+ aggiunge un chip ECS Agnus, 1 MB di Chip RAM e una ROM 2.0 all'A500. Molti giochi e demo dell'A500 non funzionano correttamente su un A500+.\nConfigurazione espansa con chip RAM da 2 MB\n\nConfigurazione espansa con RAM veloce da 4 MB\n</t>
-  </si>
-  <si>
     <t>Basic non-expanded configuration\nThe A600 is smaller than the A500+ and has an updated 2.0 ROM.\n2 MB Chip RAM expanded configuration\n\n4 MB Fast RAM expanded configuration\n</t>
   </si>
   <si>
@@ -1754,13 +1751,352 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>Dialog</t>
+  </si>
+  <si>
+    <t>System ROM Settings</t>
+  </si>
+  <si>
+    <t>Alt translation</t>
+  </si>
+  <si>
+    <t>Uscite</t>
+  </si>
+  <si>
+    <t>Ingressi</t>
+  </si>
+  <si>
+    <t>Schermi</t>
+  </si>
+  <si>
+    <t>Informazioni</t>
+  </si>
+  <si>
+    <t>Miscellanea</t>
+  </si>
+  <si>
+    <t>Chipse</t>
+  </si>
+  <si>
+    <t>Priorita &amp; Estensioni</t>
+  </si>
+  <si>
+    <t>Configurazione di base non espansa\nL'A500+ aggiunge un chip ECS Agnus, 1 MB di Chip RAM e una ROM 2.0 all'A500. Molti giochi e demo dell'A500 non funzionano correttamente su un A500+.\nConfigurazione espansa con chip RAM da 2 MB\n\nConfigurazione espansa con 4 MB di Fast RAM \n</t>
+  </si>
+  <si>
+    <t>Porte giochi</t>
+  </si>
+  <si>
+    <t>Info hardware</t>
+  </si>
+  <si>
+    <t>Swapper dischi</t>
+  </si>
+  <si>
+    <t>DeepL Translate: The world's most accurate translator</t>
+  </si>
+  <si>
+    <t>Impostazioni della ROM di sistema</t>
+  </si>
+  <si>
+    <t>Main ROM file</t>
+  </si>
+  <si>
+    <t>File ROM principale</t>
+  </si>
+  <si>
+    <t>Extended ROM file</t>
+  </si>
+  <si>
+    <t>File ROM esteso</t>
+  </si>
+  <si>
+    <t>MapROM emulation [] Creates a BlizKick-compatible memory area.</t>
+  </si>
+  <si>
+    <t>Emulazione MapROM [] Crea un'area di memoria compatibile con BlizKick.</t>
+  </si>
+  <si>
+    <t>ShapeShifter support [] Patches the system ROM for ShapeShifter compatibility.</t>
+  </si>
+  <si>
+    <t>Supporto ShapeShifter [] Rattoppa la ROM di sistema per la compatibilità con ShapeShifter.</t>
+  </si>
+  <si>
+    <t>Advanced custom ROM settings</t>
+  </si>
+  <si>
+    <t>Impostazioni avanzate della ROM personalizzata</t>
+  </si>
+  <si>
+    <t>Address range</t>
+  </si>
+  <si>
+    <t>Gamma di indirizzi</t>
+  </si>
+  <si>
+    <t>Cartridge ROM file:</t>
+  </si>
+  <si>
+    <t>File ROM della cartuccia:</t>
+  </si>
+  <si>
+    <t>Flash RAM or A2286/A2386SX BIOS CMOS RAM file:</t>
+  </si>
+  <si>
+    <t>Flash RAM o A2286/A2386SX BIOS CMOS RAM file:</t>
+  </si>
+  <si>
+    <t>Real Time Clock file</t>
+  </si>
+  <si>
+    <t>File orologio in tempo reale</t>
+  </si>
+  <si>
+    <t>Advanced UAE expansion board/Boot ROM Settings</t>
+  </si>
+  <si>
+    <t>Impostazioni avanzate della scheda di espansione UAE/Boot ROM</t>
+  </si>
+  <si>
+    <t>Tipo di scheda</t>
+  </si>
+  <si>
+    <t>Board type:</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Full Screen</t>
+  </si>
+  <si>
+    <t>Window Resize</t>
+  </si>
+  <si>
+    <t>VRR Monitor. Do not tick!</t>
+  </si>
+  <si>
+    <t>Blacker than black [] Borderblanked black is blacker than display area black.</t>
+  </si>
+  <si>
+    <t>Filtered low resolution [] When scaling hires to lores or superhires to hires, show average color of pixel instead of dropping every other pixel.</t>
+  </si>
+  <si>
+    <t>Remove interlace artifacts [] Emulates interlace mode internally as progressive, removing all interlace artifacts. Not compatible with all software.</t>
+  </si>
+  <si>
+    <t>VGA mode resolution autoswitch [] Automatically selects between hires and superhires in programmed display modes, keeping correct aspect ratio.</t>
+  </si>
+  <si>
+    <t>Monochrome video out</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>Overscan</t>
+  </si>
+  <si>
+    <t>Resolution auto switch</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>FPS adj.</t>
+  </si>
+  <si>
+    <t>Reset to defaults</t>
+  </si>
+  <si>
+    <t>Schermo</t>
+  </si>
+  <si>
+    <t>Ridimensionamento della finestra</t>
+  </si>
+  <si>
+    <t>Monitor VRR. Non spuntare!</t>
+  </si>
+  <si>
+    <t>Più nero del nero [] Il nero al limite è più nero del nero dell'area di visualizzazione.</t>
+  </si>
+  <si>
+    <t>Bassa risoluzione filtrata [] Quando si scalano le assunzioni ai lores o i superhires alle assunzioni, mostra il colore medio del pixel invece di far cadere ogni altro pixel.</t>
+  </si>
+  <si>
+    <t>Remove interlace artifacts [] Emula internamente la modalità interlacciata come progressiva, rimuovendo tutti gli artefatti di interlacciatura. Non compatibile con tutti i software.</t>
+  </si>
+  <si>
+    <t>VGA mode resolution autoswitch [] Seleziona automaticamente tra hires e superhires nelle modalità di visualizzazione programmate, mantenendo il corretto aspect ratio.</t>
+  </si>
+  <si>
+    <t>Uscita video monocromatica</t>
+  </si>
+  <si>
+    <t>Risoluzione</t>
+  </si>
+  <si>
+    <t>Commutazione automatica della risoluzione</t>
+  </si>
+  <si>
+    <t>Aggiorna</t>
+  </si>
+  <si>
+    <t>Ripristinare le impostazioni predefinite</t>
+  </si>
+  <si>
+    <t>Centering</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>Line mode</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>Scanlines</t>
+  </si>
+  <si>
+    <t>Double, fields</t>
+  </si>
+  <si>
+    <t>Double, fields+</t>
+  </si>
+  <si>
+    <t>Interlaced line mode</t>
+  </si>
+  <si>
+    <t>Centraggio</t>
+  </si>
+  <si>
+    <t>Orizzontale</t>
+  </si>
+  <si>
+    <t>Verticale</t>
+  </si>
+  <si>
+    <t>Modalità di linea</t>
+  </si>
+  <si>
+    <t>Singolo</t>
+  </si>
+  <si>
+    <t>Doppio</t>
+  </si>
+  <si>
+    <t>Double frames</t>
+  </si>
+  <si>
+    <t>Doppio, campi</t>
+  </si>
+  <si>
+    <t>Doppio, campi+</t>
+  </si>
+  <si>
+    <t>Modalità linea interlacciata</t>
+  </si>
+  <si>
+    <t>Memory Settings</t>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>Z2 Fast</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Z3 Fast</t>
+  </si>
+  <si>
+    <t>32-bit Chip</t>
+  </si>
+  <si>
+    <t>Advanced Memory Settings</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Autoconfig data</t>
+  </si>
+  <si>
+    <t>Memory board</t>
+  </si>
+  <si>
+    <t>Edit Autoconfig data</t>
+  </si>
+  <si>
+    <t>Manual configuration</t>
+  </si>
+  <si>
+    <t>DMA Capable</t>
+  </si>
+  <si>
+    <t>Force 16-bit</t>
+  </si>
+  <si>
+    <t>Z3 mapping mode</t>
+  </si>
+  <si>
+    <t>Impostazioni della memoria</t>
+  </si>
+  <si>
+    <t>Z2 Veloce</t>
+  </si>
+  <si>
+    <t>Z3 Veloce</t>
+  </si>
+  <si>
+    <t>Impostazioni avanzate della memoria</t>
+  </si>
+  <si>
+    <t>Produttore</t>
+  </si>
+  <si>
+    <t>Dati di autoconfig</t>
+  </si>
+  <si>
+    <t>Scheda di memoria</t>
+  </si>
+  <si>
+    <t>Modifica dei dati di Autoconfig</t>
+  </si>
+  <si>
+    <t>Configurazione manuale</t>
+  </si>
+  <si>
+    <t>Capacità DMA</t>
+  </si>
+  <si>
+    <t>Forza 16-bit</t>
+  </si>
+  <si>
+    <t>Modalità di mappatura Z3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1783,6 +2119,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1801,10 +2145,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1812,8 +2157,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2126,20 +2473,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:C312"/>
+  <dimension ref="A1:F378"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="A313" sqref="A313"/>
+    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="B378" sqref="B378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="105.5703125" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2149,8 +2496,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>574</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2161,7 +2514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -2172,8 +2525,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>3</v>
@@ -2184,8 +2540,11 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+1</f>
         <v>4</v>
@@ -2197,7 +2556,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A63" si="0">A5+1</f>
         <v>5</v>
@@ -2209,7 +2568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2220,8 +2579,11 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2233,7 +2595,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2244,8 +2606,11 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2257,7 +2622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2268,8 +2633,11 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2281,7 +2649,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2293,7 +2661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2304,8 +2672,11 @@
       <c r="C14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2316,8 +2687,11 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2329,7 +2703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2340,8 +2714,11 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2353,7 +2730,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2365,7 +2742,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2377,7 +2754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2389,7 +2766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2400,8 +2777,11 @@
       <c r="C22" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2413,7 +2793,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2425,7 +2805,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2436,8 +2816,11 @@
       <c r="C25" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>100</v>
       </c>
@@ -2448,7 +2831,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>101</v>
@@ -2460,7 +2843,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>102</v>
@@ -2472,7 +2855,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>103</v>
@@ -2484,7 +2867,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>104</v>
@@ -2496,7 +2879,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>105</v>
@@ -2508,7 +2891,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>106</v>
@@ -5688,7 +6071,7 @@
         <v>549</v>
       </c>
       <c r="C298" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -5697,10 +6080,10 @@
         <v>1002</v>
       </c>
       <c r="B299" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C299" t="s">
-        <v>550</v>
+        <v>582</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -5709,10 +6092,10 @@
         <v>1003</v>
       </c>
       <c r="B300" t="s">
+        <v>550</v>
+      </c>
+      <c r="C300" t="s">
         <v>551</v>
-      </c>
-      <c r="C300" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -5721,10 +6104,10 @@
         <v>1004</v>
       </c>
       <c r="B301" t="s">
+        <v>554</v>
+      </c>
+      <c r="C301" t="s">
         <v>555</v>
-      </c>
-      <c r="C301" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -5733,10 +6116,10 @@
         <v>1005</v>
       </c>
       <c r="B302" t="s">
+        <v>556</v>
+      </c>
+      <c r="C302" t="s">
         <v>557</v>
-      </c>
-      <c r="C302" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -5745,10 +6128,10 @@
         <v>1006</v>
       </c>
       <c r="B303" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C303" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -5757,91 +6140,621 @@
         <v>1007</v>
       </c>
       <c r="B304" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C304" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305">
         <f t="shared" si="3"/>
         <v>1008</v>
       </c>
       <c r="B305" t="s">
+        <v>562</v>
+      </c>
+      <c r="C305" t="s">
         <v>563</v>
       </c>
-      <c r="C305" t="s">
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <f t="shared" ref="A306:A310" si="4">A305+1</f>
+        <v>1009</v>
+      </c>
+      <c r="B306" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A306">
-        <f t="shared" ref="A306:A313" si="4">A305+1</f>
-        <v>1009</v>
-      </c>
-      <c r="B306" t="s">
+      <c r="C306" t="s">
         <v>565</v>
       </c>
-      <c r="C306" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307">
         <f t="shared" si="4"/>
         <v>1010</v>
       </c>
       <c r="B307" t="s">
+        <v>566</v>
+      </c>
+      <c r="C307" t="s">
         <v>567</v>
       </c>
-      <c r="C307" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308">
         <f t="shared" si="4"/>
         <v>1011</v>
       </c>
       <c r="B308" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C308" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309">
         <f t="shared" si="4"/>
         <v>1012</v>
       </c>
       <c r="B309" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C309" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310">
         <f t="shared" si="4"/>
         <v>1013</v>
       </c>
       <c r="B310" t="s">
+        <v>570</v>
+      </c>
+      <c r="C310" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
         <v>571</v>
       </c>
-      <c r="C310" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
+      <c r="E312" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>572</v>
       </c>
     </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>107</v>
+      </c>
+      <c r="B315" t="s">
+        <v>573</v>
+      </c>
+      <c r="C315" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>588</v>
+      </c>
+      <c r="C316" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>590</v>
+      </c>
+      <c r="C317" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>592</v>
+      </c>
+      <c r="C318" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>594</v>
+      </c>
+      <c r="C319" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>596</v>
+      </c>
+      <c r="C320" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B321" t="s">
+        <v>598</v>
+      </c>
+      <c r="C321" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>14</v>
+      </c>
+      <c r="C322" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>600</v>
+      </c>
+      <c r="C323" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B324" t="s">
+        <v>602</v>
+      </c>
+      <c r="C324" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>604</v>
+      </c>
+      <c r="C325" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>606</v>
+      </c>
+      <c r="C326" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>609</v>
+      </c>
+      <c r="C327" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>108</v>
+      </c>
+      <c r="B328" t="s">
+        <v>610</v>
+      </c>
+      <c r="C328" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>611</v>
+      </c>
+      <c r="C329" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>203</v>
+      </c>
+      <c r="C330" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>612</v>
+      </c>
+      <c r="C331" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>613</v>
+      </c>
+      <c r="C332" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B333" t="s">
+        <v>252</v>
+      </c>
+      <c r="C333" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>498</v>
+      </c>
+      <c r="C334" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>500</v>
+      </c>
+      <c r="C335" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>614</v>
+      </c>
+      <c r="C336" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="337" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
+        <v>615</v>
+      </c>
+      <c r="C337" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="338" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>616</v>
+      </c>
+      <c r="C338" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="339" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>617</v>
+      </c>
+      <c r="C339" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="340" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>618</v>
+      </c>
+      <c r="C340" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="341" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B341" t="s">
+        <v>619</v>
+      </c>
+      <c r="C341" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="342" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B342" t="s">
+        <v>620</v>
+      </c>
+      <c r="C342" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="343" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
+        <v>621</v>
+      </c>
+      <c r="C343" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="344" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
+        <v>622</v>
+      </c>
+      <c r="C344" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="345" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
+        <v>623</v>
+      </c>
+      <c r="C345" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="346" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B346" t="s">
+        <v>624</v>
+      </c>
+      <c r="C346" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="347" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>637</v>
+      </c>
+      <c r="C347" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="348" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B348" t="s">
+        <v>638</v>
+      </c>
+      <c r="C348" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="349" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B349" t="s">
+        <v>639</v>
+      </c>
+      <c r="C349" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="350" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
+        <v>640</v>
+      </c>
+      <c r="C350" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="351" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
+        <v>641</v>
+      </c>
+      <c r="C351" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="352" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B352" t="s">
+        <v>642</v>
+      </c>
+      <c r="C352" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>643</v>
+      </c>
+      <c r="C353" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>644</v>
+      </c>
+      <c r="C354" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>645</v>
+      </c>
+      <c r="C355" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>646</v>
+      </c>
+      <c r="C356" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
+        <v>641</v>
+      </c>
+      <c r="C357" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
+        <v>653</v>
+      </c>
+      <c r="C358" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
+        <v>644</v>
+      </c>
+      <c r="C359" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
+        <v>645</v>
+      </c>
+      <c r="C360" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>109</v>
+      </c>
+      <c r="B361" t="s">
+        <v>657</v>
+      </c>
+      <c r="C361" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>658</v>
+      </c>
+      <c r="C362" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>659</v>
+      </c>
+      <c r="C363" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
+        <v>660</v>
+      </c>
+      <c r="C364" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
+        <v>661</v>
+      </c>
+      <c r="C365" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
+        <v>662</v>
+      </c>
+      <c r="C366" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
+        <v>663</v>
+      </c>
+      <c r="C367" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B368" t="s">
+        <v>664</v>
+      </c>
+      <c r="C368" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B369" t="s">
+        <v>665</v>
+      </c>
+      <c r="C369" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B370" t="s">
+        <v>666</v>
+      </c>
+      <c r="C370" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B371" t="s">
+        <v>667</v>
+      </c>
+      <c r="C371" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B372" t="s">
+        <v>598</v>
+      </c>
+      <c r="C372" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B373" t="s">
+        <v>668</v>
+      </c>
+      <c r="C373" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B374" t="s">
+        <v>669</v>
+      </c>
+      <c r="C374" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B375" t="s">
+        <v>670</v>
+      </c>
+      <c r="C375" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B376" t="s">
+        <v>671</v>
+      </c>
+      <c r="C376" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B377" t="s">
+        <v>672</v>
+      </c>
+      <c r="C377" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
+    <hyperlink ref="E312" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Translations for CPU, Contributors and Disk drive
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091BB30-43ED-4654-A643-E754DE535F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED1F377-F077-493E-8B67-CB9F3D18DA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14745" yWindow="2535" windowWidth="36465" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="13815" yWindow="690" windowWidth="28905" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="817">
   <si>
     <t>ID</t>
   </si>
@@ -2090,6 +2090,402 @@
   </si>
   <si>
     <t>Modalità di mappatura Z3</t>
+  </si>
+  <si>
+    <t>https://github.com/pjhutch17/WinuaeItalianTranslation</t>
+  </si>
+  <si>
+    <t>Floppy Drives</t>
+  </si>
+  <si>
+    <t>Delete save image</t>
+  </si>
+  <si>
+    <t>Eject</t>
+  </si>
+  <si>
+    <t>Floppy Drive Emulation Speed</t>
+  </si>
+  <si>
+    <t>New Floppy Disk Image</t>
+  </si>
+  <si>
+    <t>Create Standard Disk [] Creates a standard 880 or 1760 KB ADF disk image.</t>
+  </si>
+  <si>
+    <t>Create Custom Disk [] Creates a low level (MFM) ADF disk image (about 2MB). Useful for programs that use non-standard disk formats (for example some save disks or DOS-formatted floppies)</t>
+  </si>
+  <si>
+    <t>Disk label</t>
+  </si>
+  <si>
+    <t>Bootblock</t>
+  </si>
+  <si>
+    <t>FFS</t>
+  </si>
+  <si>
+    <t>Cancellare salvare l'immagine</t>
+  </si>
+  <si>
+    <t>Move box to X = 48</t>
+  </si>
+  <si>
+    <t>Write-protected</t>
+  </si>
+  <si>
+    <t>Protetto dalla scrittura</t>
+  </si>
+  <si>
+    <t>Espellere</t>
+  </si>
+  <si>
+    <t>Velocità di emulazione dell'unità floppy</t>
+  </si>
+  <si>
+    <t>Nuova immagine del disco floppy</t>
+  </si>
+  <si>
+    <t>Create Standard Disk [] Crea un'immagine disco ADF standard da 880 o 1760 KB.</t>
+  </si>
+  <si>
+    <t>Etichetta del disco</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>24-bit addressing</t>
+  </si>
+  <si>
+    <t>More compatible [] 68000: emulate prefetch. 68020+: emulate prefetch and instruction cache. More compatible but slower.</t>
+  </si>
+  <si>
+    <t>Data cache emulation [] 68030, 040 and 060 optional data cache emulation. Requires More compatible option.</t>
+  </si>
+  <si>
+    <t>JIT [] Enable just-in-time CPU emulator. Significantly increases the speed of the CPU emulation. Requires 68020 or higher CPU.</t>
+  </si>
+  <si>
+    <t>Unimplemented CPU emu [] Emulate 68060 unimplemented integer instructions</t>
+  </si>
+  <si>
+    <t>CPU Emulation Speed</t>
+  </si>
+  <si>
+    <t>Fastest possible</t>
+  </si>
+  <si>
+    <t>Approximate A500/A1200 or cycle-exact</t>
+  </si>
+  <si>
+    <t>CPU Speed</t>
+  </si>
+  <si>
+    <t>CPU Idle</t>
+  </si>
+  <si>
+    <t>Cycle-exact CPU Emulation Speed</t>
+  </si>
+  <si>
+    <t>CPU Frequency</t>
+  </si>
+  <si>
+    <t>PPC CPU options</t>
+  </si>
+  <si>
+    <t>PPC CPU emulation (Blizzard PPC / CyberStorm PPC) [] Automatically configure CyberStorm PPC or Blizzard PPC setup.</t>
+  </si>
+  <si>
+    <t>Stopped M68K CPU idle mode</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>MMU</t>
+  </si>
+  <si>
+    <t>MMU [] 68030, 68040 and 68060 MMU emulation. Not compatible with JIT.</t>
+  </si>
+  <si>
+    <t>EC [] 68EC030, 68EC040 and 68EC060 Transparent Translation Register emulation. Not compatible with JIT.</t>
+  </si>
+  <si>
+    <t>x86 Bridgeboard CPU options</t>
+  </si>
+  <si>
+    <t>FPU</t>
+  </si>
+  <si>
+    <t>CPU internal</t>
+  </si>
+  <si>
+    <t>More compatible [] More compatible but slower FPU emulation.</t>
+  </si>
+  <si>
+    <t>Unimplemented FPU emu [] Emulate FPU unimplemented instructions</t>
+  </si>
+  <si>
+    <t>Advanced JIT Settings</t>
+  </si>
+  <si>
+    <t>Cache size:</t>
+  </si>
+  <si>
+    <t>FPU support</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Catch unexpected exceptions</t>
+  </si>
+  <si>
+    <t>Constant jump</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>Hard flush</t>
+  </si>
+  <si>
+    <t>No flags</t>
+  </si>
+  <si>
+    <t>Più compatibile [] 68000: emula il prefetch. 68020+: emula il prefetch e la cache delle istruzioni. Più compatibile ma più lento.</t>
+  </si>
+  <si>
+    <t>Indirizzamento a 24 bit</t>
+  </si>
+  <si>
+    <t>Emulazione cache dati [] 68030, 040 e 060 emulazione cache dati opzionale. Richiede un'opzione più compatibile.</t>
+  </si>
+  <si>
+    <t>JIT [] Abilita l'emulatore di CPU just-in-time. Aumenta significativamente la velocità dell'emulazione della CPU. Richiede una CPU 68020 o superiore.</t>
+  </si>
+  <si>
+    <t>CPU non implementata emu [] Emula istruzioni intere non implementate 68060</t>
+  </si>
+  <si>
+    <t>Il più veloce possibile</t>
+  </si>
+  <si>
+    <t>Approssimativo A500/A1200 o ciclo-esatto</t>
+  </si>
+  <si>
+    <t>Velocità di emulazione della CPU</t>
+  </si>
+  <si>
+    <t>CPU Velocità</t>
+  </si>
+  <si>
+    <t>CPU inattiva</t>
+  </si>
+  <si>
+    <t>Velocità di emulazione della CPU Cycle-exact</t>
+  </si>
+  <si>
+    <t>Frequenza della CPU</t>
+  </si>
+  <si>
+    <t>Opzioni CPU PPC</t>
+  </si>
+  <si>
+    <t>Emulazione CPU PPC (Blizzard PPC / CyberStorm PPC) [] Configura automaticamente la configurazione CyberStorm PPC o Blizzard PPC.</t>
+  </si>
+  <si>
+    <t>Arresto della modalità inattiva della CPU M68K</t>
+  </si>
+  <si>
+    <t>Nessuno</t>
+  </si>
+  <si>
+    <t>MMU [] Emulazione MMU 68030, 68040 e 68060. Non compatibile con JIT.</t>
+  </si>
+  <si>
+    <t>EC [] 68EC030, 68EC040 e 68EC060 Emulazione del registro di traduzione trasparente. Non compatibile con JIT.</t>
+  </si>
+  <si>
+    <t>Opzioni CPU x86 Bridgeboard</t>
+  </si>
+  <si>
+    <t>Velocità della CPU</t>
+  </si>
+  <si>
+    <t>Interno della CPU</t>
+  </si>
+  <si>
+    <t>Più compatibile [] Emulazione FPU più compatibile ma più lenta.</t>
+  </si>
+  <si>
+    <t>Unimplemented FPU emu [] Emula istruzioni FPU non implementate</t>
+  </si>
+  <si>
+    <t>Dimensione della cache:</t>
+  </si>
+  <si>
+    <t>Impostazioni JIT avanzate</t>
+  </si>
+  <si>
+    <t>Supporto FPU</t>
+  </si>
+  <si>
+    <t>Diretto</t>
+  </si>
+  <si>
+    <t>Cattura le eccezioni inaspettate</t>
+  </si>
+  <si>
+    <t>Salto costante</t>
+  </si>
+  <si>
+    <t>Indiretto</t>
+  </si>
+  <si>
+    <t>Sciacquone duro</t>
+  </si>
+  <si>
+    <t>Nessuna bandiera</t>
+  </si>
+  <si>
+    <t>Contributers</t>
+  </si>
+  <si>
+    <t>Collaboratori</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Item1 - Item6</t>
+  </si>
+  <si>
+    <t>Add SCSI/IDE CD Drive</t>
+  </si>
+  <si>
+    <t>Add SCSI/IDE Tape Drive</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Add PC drives at startup</t>
+  </si>
+  <si>
+    <t>CDFS automount CD/DVD drives</t>
+  </si>
+  <si>
+    <t>Disable UAEFSDB-support</t>
+  </si>
+  <si>
+    <t>Don't use Windows Recycle Bin</t>
+  </si>
+  <si>
+    <t>Automount removable drives [] Windows side insert or removal will immediately mount/remove it on Amiga side.</t>
+  </si>
+  <si>
+    <t>Limit size of directory drives to 1G [] Workaround for example old installers that calculate free space incorrectly if drive is large.</t>
+  </si>
+  <si>
+    <t>Optical media options</t>
+  </si>
+  <si>
+    <t>CD drive/image</t>
+  </si>
+  <si>
+    <t>Select image file</t>
+  </si>
+  <si>
+    <t>Titolo</t>
+  </si>
+  <si>
+    <t>Aggiungere una directory o un archivio</t>
+  </si>
+  <si>
+    <t>Add &amp;Directory or Archive</t>
+  </si>
+  <si>
+    <t>Aggiungi &amp;Hardfile</t>
+  </si>
+  <si>
+    <t>Add &amp;Hardfile…</t>
+  </si>
+  <si>
+    <t>Add H&amp;ard Drive...</t>
+  </si>
+  <si>
+    <t>Aggiungi H&amp;ard Drive...</t>
+  </si>
+  <si>
+    <t>Aggiungere unità CD SCSI/IDE</t>
+  </si>
+  <si>
+    <t>Aggiungere unità a nastro SCSI/IDE</t>
+  </si>
+  <si>
+    <t>&amp;Properties</t>
+  </si>
+  <si>
+    <t>Rimuovi</t>
+  </si>
+  <si>
+    <t>&amp;Proprietà</t>
+  </si>
+  <si>
+    <t>Opzioni</t>
+  </si>
+  <si>
+    <t>Aggiungere unità PC all'avvio</t>
+  </si>
+  <si>
+    <t>Includere unità rimovibili..</t>
+  </si>
+  <si>
+    <t>Include removable drives..</t>
+  </si>
+  <si>
+    <t>Include network drives..</t>
+  </si>
+  <si>
+    <t>Includere le unità di rete..</t>
+  </si>
+  <si>
+    <t>CDFS monta automaticamente le unità CD/DVD</t>
+  </si>
+  <si>
+    <t>Disattivare il supporto UAEFSDB</t>
+  </si>
+  <si>
+    <t>Non usare il Cestino di Windows</t>
+  </si>
+  <si>
+    <t>Automount dei drive rimovibili [] L'inserimento o la rimozione dal lato Windows lo monta/rimuove immediatamente sul lato Amiga.</t>
+  </si>
+  <si>
+    <t>Limitare la dimensione delle unità di directory a 1G [] Soluzione per esempio per vecchi installatori che calcolano erroneamente lo spazio libero se l'unità è grande.</t>
+  </si>
+  <si>
+    <t>Opzioni dei supporti ottici</t>
+  </si>
+  <si>
+    <t>Unità CD/immagine</t>
+  </si>
+  <si>
+    <t>Seleziona il file immagine</t>
+  </si>
+  <si>
+    <t>CDTV/CDTV-CR/CD32 turbo CD read speed</t>
+  </si>
+  <si>
+    <t>Velocità di lettura CDTV/CDTV-CR/CD32 turbo CD</t>
+  </si>
+  <si>
+    <t>Voce1</t>
   </si>
 </sst>
 </file>
@@ -2473,10 +2869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F378"/>
+  <dimension ref="A1:F448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="B378" sqref="B378"/>
+    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
+      <selection activeCell="B428" sqref="B428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6222,14 +6618,14 @@
       <c r="A312" t="s">
         <v>571</v>
       </c>
-      <c r="E312" s="5" t="s">
-        <v>586</v>
-      </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>572</v>
       </c>
+      <c r="E314" s="5" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315">
@@ -6672,7 +7068,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
         <v>665</v>
       </c>
@@ -6680,7 +7076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
         <v>666</v>
       </c>
@@ -6688,7 +7084,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
         <v>667</v>
       </c>
@@ -6696,7 +7092,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
         <v>598</v>
       </c>
@@ -6704,7 +7100,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
         <v>668</v>
       </c>
@@ -6712,7 +7108,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
         <v>669</v>
       </c>
@@ -6720,7 +7116,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
         <v>670</v>
       </c>
@@ -6728,7 +7124,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
         <v>671</v>
       </c>
@@ -6736,7 +7132,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
         <v>672</v>
       </c>
@@ -6744,17 +7140,596 @@
         <v>684</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>110</v>
+      </c>
+      <c r="B378" t="s">
+        <v>686</v>
+      </c>
+      <c r="C378" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B379" t="s">
+        <v>687</v>
+      </c>
+      <c r="C379" t="s">
+        <v>696</v>
+      </c>
+      <c r="D379" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B380" t="s">
+        <v>698</v>
+      </c>
+      <c r="C380" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B381" t="s">
+        <v>688</v>
+      </c>
+      <c r="C381" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B382" t="s">
+        <v>689</v>
+      </c>
+      <c r="C382" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B383" t="s">
+        <v>690</v>
+      </c>
+      <c r="C383" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B384" t="s">
+        <v>691</v>
+      </c>
+      <c r="C384" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B385" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B386" t="s">
+        <v>693</v>
+      </c>
+      <c r="C386" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B387" t="s">
+        <v>694</v>
+      </c>
+      <c r="C387" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B388" t="s">
+        <v>695</v>
+      </c>
+      <c r="C388" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>111</v>
+      </c>
+      <c r="B389" t="s">
+        <v>705</v>
+      </c>
+      <c r="C389" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B390" t="s">
+        <v>706</v>
+      </c>
+      <c r="C390" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B391" t="s">
+        <v>707</v>
+      </c>
+      <c r="C391" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B392" t="s">
+        <v>708</v>
+      </c>
+      <c r="C392" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B393" t="s">
+        <v>709</v>
+      </c>
+      <c r="C393" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B394" t="s">
+        <v>710</v>
+      </c>
+      <c r="C394" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B395" t="s">
+        <v>711</v>
+      </c>
+      <c r="C395" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B396" t="s">
+        <v>712</v>
+      </c>
+      <c r="C396" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B397" t="s">
+        <v>713</v>
+      </c>
+      <c r="C397" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B398" t="s">
+        <v>714</v>
+      </c>
+      <c r="C398" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B399" t="s">
+        <v>715</v>
+      </c>
+      <c r="C399" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B400" t="s">
+        <v>716</v>
+      </c>
+      <c r="C400" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="401" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B401" t="s">
+        <v>717</v>
+      </c>
+      <c r="C401" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="402" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B402" t="s">
+        <v>718</v>
+      </c>
+      <c r="C402" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="403" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B403" t="s">
+        <v>719</v>
+      </c>
+      <c r="C403" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="404" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B404" t="s">
+        <v>720</v>
+      </c>
+      <c r="C404" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="405" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B405" t="s">
+        <v>722</v>
+      </c>
+      <c r="C405" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="406" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B406" t="s">
+        <v>721</v>
+      </c>
+      <c r="C406" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="407" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B407" t="s">
+        <v>723</v>
+      </c>
+      <c r="C407" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="408" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B408" t="s">
+        <v>724</v>
+      </c>
+      <c r="C408" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="409" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B409" t="s">
+        <v>725</v>
+      </c>
+      <c r="C409" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="410" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B410" t="s">
+        <v>714</v>
+      </c>
+      <c r="C410" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="411" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B411" t="s">
+        <v>726</v>
+      </c>
+      <c r="C411" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="412" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B412" t="s">
+        <v>721</v>
+      </c>
+      <c r="C412" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="413" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B413" t="s">
+        <v>727</v>
+      </c>
+      <c r="C413" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="414" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B414" t="s">
+        <v>728</v>
+      </c>
+      <c r="C414" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="415" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B415" t="s">
+        <v>729</v>
+      </c>
+      <c r="C415" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="416" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B416" t="s">
+        <v>730</v>
+      </c>
+      <c r="C416" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B417" t="s">
+        <v>731</v>
+      </c>
+      <c r="C417" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B418" t="s">
+        <v>732</v>
+      </c>
+      <c r="C418" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B419" t="s">
+        <v>733</v>
+      </c>
+      <c r="C419" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B420" t="s">
+        <v>734</v>
+      </c>
+      <c r="C420" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B421" t="s">
+        <v>735</v>
+      </c>
+      <c r="C421" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B422" t="s">
+        <v>736</v>
+      </c>
+      <c r="C422" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B423" t="s">
+        <v>737</v>
+      </c>
+      <c r="C423" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B424" t="s">
+        <v>738</v>
+      </c>
+      <c r="C424" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>112</v>
+      </c>
+      <c r="B425" t="s">
+        <v>771</v>
+      </c>
+      <c r="C425" t="s">
+        <v>772</v>
+      </c>
+      <c r="D425" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>113</v>
+      </c>
+      <c r="B426" t="s">
+        <v>773</v>
+      </c>
+      <c r="C426" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B427" t="s">
+        <v>774</v>
+      </c>
+      <c r="C427" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B428" t="s">
+        <v>790</v>
+      </c>
+      <c r="C428" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B429" t="s">
+        <v>792</v>
+      </c>
+      <c r="C429" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B430" t="s">
+        <v>793</v>
+      </c>
+      <c r="C430" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B431" t="s">
+        <v>775</v>
+      </c>
+      <c r="C431" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B432" t="s">
+        <v>776</v>
+      </c>
+      <c r="C432" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="433" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B433" t="s">
+        <v>797</v>
+      </c>
+      <c r="C433" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="434" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B434" t="s">
+        <v>777</v>
+      </c>
+      <c r="C434" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="435" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B435" t="s">
+        <v>778</v>
+      </c>
+      <c r="C435" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="436" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B436" t="s">
+        <v>779</v>
+      </c>
+      <c r="C436" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="437" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B437" t="s">
+        <v>803</v>
+      </c>
+      <c r="C437" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="438" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B438" t="s">
+        <v>804</v>
+      </c>
+      <c r="C438" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="439" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B439" t="s">
+        <v>780</v>
+      </c>
+      <c r="C439" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="440" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B440" t="s">
+        <v>781</v>
+      </c>
+      <c r="C440" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="441" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B441" t="s">
+        <v>782</v>
+      </c>
+      <c r="C441" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="442" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B442" t="s">
+        <v>783</v>
+      </c>
+      <c r="C442" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="443" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B443" t="s">
+        <v>784</v>
+      </c>
+      <c r="C443" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="444" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B444" t="s">
+        <v>785</v>
+      </c>
+      <c r="C444" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="445" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B445" t="s">
+        <v>786</v>
+      </c>
+      <c r="C445" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="446" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B446" t="s">
+        <v>787</v>
+      </c>
+      <c r="C446" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="447" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B447" t="s">
+        <v>688</v>
+      </c>
+      <c r="C447" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="448" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B448" t="s">
+        <v>814</v>
+      </c>
+      <c r="C448" t="s">
+        <v>815</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="E312" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D425" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sound and ports translations added
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED1F377-F077-493E-8B67-CB9F3D18DA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2D79F7-483C-49A7-B240-C47C70D5D082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="690" windowWidth="28905" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="15915" yWindow="555" windowWidth="21645" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="895">
   <si>
     <t>ID</t>
   </si>
@@ -2486,6 +2486,240 @@
   </si>
   <si>
     <t>Voce1</t>
+  </si>
+  <si>
+    <t>Sound Emulation</t>
+  </si>
+  <si>
+    <t>Disabled, but emulated</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Automatic switching</t>
+  </si>
+  <si>
+    <t>Include CD and FMV audio</t>
+  </si>
+  <si>
+    <t>Volume Counter mode</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Sound Buffer Size</t>
+  </si>
+  <si>
+    <t>Channel mode:</t>
+  </si>
+  <si>
+    <t>Stereo separation:</t>
+  </si>
+  <si>
+    <t>Interpolation:</t>
+  </si>
+  <si>
+    <t>Frequency:</t>
+  </si>
+  <si>
+    <t>Swap channels:</t>
+  </si>
+  <si>
+    <t>Stereo delay:</t>
+  </si>
+  <si>
+    <t>Audio filter:</t>
+  </si>
+  <si>
+    <t>Floppy Drive Sound Emulation</t>
+  </si>
+  <si>
+    <t>Empty drive</t>
+  </si>
+  <si>
+    <t>Disk in drive</t>
+  </si>
+  <si>
+    <t>Drivers</t>
+  </si>
+  <si>
+    <t>DirectSound</t>
+  </si>
+  <si>
+    <t>WASAPI</t>
+  </si>
+  <si>
+    <t>OpenAL</t>
+  </si>
+  <si>
+    <t>PortAudio</t>
+  </si>
+  <si>
+    <t>Emulazione del suono</t>
+  </si>
+  <si>
+    <t>Disabilitato, ma emulato</t>
+  </si>
+  <si>
+    <t>Abilitato</t>
+  </si>
+  <si>
+    <t>Commutazione automatica</t>
+  </si>
+  <si>
+    <t>Include CD e audio FMV</t>
+  </si>
+  <si>
+    <t>Modalità del contatore di volume</t>
+  </si>
+  <si>
+    <t>Dimensione del buffer sonoro</t>
+  </si>
+  <si>
+    <t>Modalità di canale:</t>
+  </si>
+  <si>
+    <t>Separazione stereo:</t>
+  </si>
+  <si>
+    <t>Interpolazione:</t>
+  </si>
+  <si>
+    <t>Frequenza:</t>
+  </si>
+  <si>
+    <t>Scambiare i canali:</t>
+  </si>
+  <si>
+    <t>Ritardo stereo:</t>
+  </si>
+  <si>
+    <t>Filtro audio:</t>
+  </si>
+  <si>
+    <t>Emulazione sonora dell'unità floppy</t>
+  </si>
+  <si>
+    <t>Disco vuoto</t>
+  </si>
+  <si>
+    <t>Disco nel drive</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Expand item</t>
+  </si>
+  <si>
+    <t>Leaf</t>
+  </si>
+  <si>
+    <t>Collapse Item</t>
+  </si>
+  <si>
+    <t>Parallel Port</t>
+  </si>
+  <si>
+    <t>Flush print job</t>
+  </si>
+  <si>
+    <t>Autoflush [] Time in seconds after a pending print job is automatically flushed.</t>
+  </si>
+  <si>
+    <t>Ghostscript extra parameters:</t>
+  </si>
+  <si>
+    <t>Stereo sampler</t>
+  </si>
+  <si>
+    <t>Serial Port</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>RTS/CTS</t>
+  </si>
+  <si>
+    <t>Direct []Use when emulating serial-link games on two PCs running WinUAE</t>
+  </si>
+  <si>
+    <t>uaeserial.device</t>
+  </si>
+  <si>
+    <t>MIDI</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>Route MIDI In to MIDI Out</t>
+  </si>
+  <si>
+    <t>Protection Dongle</t>
+  </si>
+  <si>
+    <t>Porta parallela</t>
+  </si>
+  <si>
+    <t>Stampante</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Risciacquo del lavoro di stampa</t>
+  </si>
+  <si>
+    <t>Autoflush [] Tempo in secondi dopo il lavaggio automatico di un lavoro di stampa in attesa.</t>
+  </si>
+  <si>
+    <t>Printer:</t>
+  </si>
+  <si>
+    <t>Type:</t>
+  </si>
+  <si>
+    <t>Sampler:</t>
+  </si>
+  <si>
+    <t>Parametri extra di Ghostscript:</t>
+  </si>
+  <si>
+    <t>Campionario:</t>
+  </si>
+  <si>
+    <t>Campionatore stereo</t>
+  </si>
+  <si>
+    <t>Porta seriale</t>
+  </si>
+  <si>
+    <t>Condiviso</t>
+  </si>
+  <si>
+    <t>Fuori</t>
+  </si>
+  <si>
+    <t>Direct []Da utilizzare per l'emulazione di giochi con collegamento seriale su due PC con WinUAE.</t>
+  </si>
+  <si>
+    <t>Indirizzare l'ingresso MIDI all'uscita MIDI</t>
+  </si>
+  <si>
+    <t>Dongle di protezione</t>
+  </si>
+  <si>
+    <t>UAE Authors and Contributors...</t>
+  </si>
+  <si>
+    <t>Autori e collaboratori degli Emirati Arabi Uniti...</t>
   </si>
 </sst>
 </file>
@@ -2869,10 +3103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F448"/>
+  <dimension ref="A1:F497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="B428" sqref="B428"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="A498" sqref="A498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7458,7 +7692,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
         <v>731</v>
       </c>
@@ -7466,7 +7700,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
         <v>732</v>
       </c>
@@ -7474,7 +7708,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
         <v>733</v>
       </c>
@@ -7482,7 +7716,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
         <v>734</v>
       </c>
@@ -7490,7 +7724,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
         <v>735</v>
       </c>
@@ -7498,7 +7732,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
         <v>736</v>
       </c>
@@ -7506,7 +7740,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
         <v>737</v>
       </c>
@@ -7514,7 +7748,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
         <v>738</v>
       </c>
@@ -7522,7 +7756,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>112</v>
       </c>
@@ -7532,11 +7766,8 @@
       <c r="C425" t="s">
         <v>772</v>
       </c>
-      <c r="D425" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>113</v>
       </c>
@@ -7547,7 +7778,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
         <v>774</v>
       </c>
@@ -7555,7 +7786,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
         <v>790</v>
       </c>
@@ -7563,7 +7794,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
         <v>792</v>
       </c>
@@ -7571,7 +7802,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
         <v>793</v>
       </c>
@@ -7579,7 +7810,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
         <v>775</v>
       </c>
@@ -7587,7 +7818,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
         <v>776</v>
       </c>
@@ -7723,10 +7954,408 @@
         <v>815</v>
       </c>
     </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>122</v>
+      </c>
+      <c r="B449" t="s">
+        <v>817</v>
+      </c>
+      <c r="C449" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B450" t="s">
+        <v>215</v>
+      </c>
+      <c r="C450" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B451" t="s">
+        <v>818</v>
+      </c>
+      <c r="C451" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B452" t="s">
+        <v>819</v>
+      </c>
+      <c r="C452" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B453" t="s">
+        <v>820</v>
+      </c>
+      <c r="C453" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B454" t="s">
+        <v>821</v>
+      </c>
+      <c r="C454" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B455" t="s">
+        <v>822</v>
+      </c>
+      <c r="C455" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B456" t="s">
+        <v>96</v>
+      </c>
+      <c r="C456" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B457" t="s">
+        <v>823</v>
+      </c>
+      <c r="C457" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B458" t="s">
+        <v>824</v>
+      </c>
+      <c r="C458" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B459" t="s">
+        <v>252</v>
+      </c>
+      <c r="C459" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B460" t="s">
+        <v>825</v>
+      </c>
+      <c r="C460" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B461" t="s">
+        <v>826</v>
+      </c>
+      <c r="C461" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B462" t="s">
+        <v>827</v>
+      </c>
+      <c r="C462" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B463" t="s">
+        <v>828</v>
+      </c>
+      <c r="C463" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B464" t="s">
+        <v>829</v>
+      </c>
+      <c r="C464" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B465" t="s">
+        <v>830</v>
+      </c>
+      <c r="C465" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B466" t="s">
+        <v>831</v>
+      </c>
+      <c r="C466" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B467" t="s">
+        <v>832</v>
+      </c>
+      <c r="C467" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B468" t="s">
+        <v>833</v>
+      </c>
+      <c r="C468" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B469" t="s">
+        <v>834</v>
+      </c>
+      <c r="C469" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B470" t="s">
+        <v>835</v>
+      </c>
+      <c r="C470" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B471" t="s">
+        <v>836</v>
+      </c>
+      <c r="C471" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B472" t="s">
+        <v>837</v>
+      </c>
+      <c r="C472" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B473" t="s">
+        <v>838</v>
+      </c>
+      <c r="C473" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B474" t="s">
+        <v>839</v>
+      </c>
+      <c r="C474" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>135</v>
+      </c>
+      <c r="B475" t="s">
+        <v>858</v>
+      </c>
+      <c r="D475" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B476" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B477" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>138</v>
+      </c>
+      <c r="B478" t="s">
+        <v>861</v>
+      </c>
+      <c r="C478" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B479" t="s">
+        <v>881</v>
+      </c>
+      <c r="C479" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B480" t="s">
+        <v>882</v>
+      </c>
+      <c r="C480" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B481" t="s">
+        <v>862</v>
+      </c>
+      <c r="C481" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B482" t="s">
+        <v>863</v>
+      </c>
+      <c r="C482" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B483" t="s">
+        <v>864</v>
+      </c>
+      <c r="C483" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B484" t="s">
+        <v>883</v>
+      </c>
+      <c r="C484" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B485" t="s">
+        <v>865</v>
+      </c>
+      <c r="C485" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B486" t="s">
+        <v>866</v>
+      </c>
+      <c r="C486" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B487" t="s">
+        <v>867</v>
+      </c>
+      <c r="C487" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B488" t="s">
+        <v>868</v>
+      </c>
+      <c r="C488" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B489" t="s">
+        <v>869</v>
+      </c>
+      <c r="C489" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B490" t="s">
+        <v>870</v>
+      </c>
+      <c r="C490" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B491" t="s">
+        <v>871</v>
+      </c>
+      <c r="C491" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B492" t="s">
+        <v>872</v>
+      </c>
+      <c r="C492" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B493" t="s">
+        <v>873</v>
+      </c>
+      <c r="C493" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B494" t="s">
+        <v>874</v>
+      </c>
+      <c r="C494" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B495" t="s">
+        <v>875</v>
+      </c>
+      <c r="C495" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>140</v>
+      </c>
+      <c r="B496" t="s">
+        <v>893</v>
+      </c>
+      <c r="C496" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>141</v>
+      </c>
+      <c r="B497" t="s">
+        <v>774</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D425" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D475" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Misc and hard drive translations
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2D79F7-483C-49A7-B240-C47C70D5D082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB194F-825B-40DB-86AB-F0680CB5DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15915" yWindow="555" windowWidth="21645" windowHeight="16620" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="9420" yWindow="1860" windowWidth="27060" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="971">
   <si>
     <t>ID</t>
   </si>
@@ -2720,13 +2720,241 @@
   </si>
   <si>
     <t>Autori e collaboratori degli Emirati Arabi Uniti...</t>
+  </si>
+  <si>
+    <t>Miscellaneous Options</t>
+  </si>
+  <si>
+    <t>SCSI and CD/DVD access:</t>
+  </si>
+  <si>
+    <t>Windowed style:</t>
+  </si>
+  <si>
+    <t>Graphics API:</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>GUI Font...</t>
+  </si>
+  <si>
+    <t>Set default</t>
+  </si>
+  <si>
+    <t>Reset list customizations</t>
+  </si>
+  <si>
+    <t>Resizeable GUI</t>
+  </si>
+  <si>
+    <t>Fullscreen GUI</t>
+  </si>
+  <si>
+    <t>State Files</t>
+  </si>
+  <si>
+    <t>Load state...</t>
+  </si>
+  <si>
+    <t>Save state...</t>
+  </si>
+  <si>
+    <t>Keyboard LEDs</t>
+  </si>
+  <si>
+    <t>USB mode</t>
+  </si>
+  <si>
+    <t>Opzioni varie</t>
+  </si>
+  <si>
+    <t>Accesso SCSI e CD/DVD:</t>
+  </si>
+  <si>
+    <t>Stile a finestra:</t>
+  </si>
+  <si>
+    <t>API grafica:</t>
+  </si>
+  <si>
+    <t>Font GUI...</t>
+  </si>
+  <si>
+    <t>Predefinita</t>
+  </si>
+  <si>
+    <t>Ripristino delle personalizzazioni dell'elenco</t>
+  </si>
+  <si>
+    <t>GUI ridimensionabile</t>
+  </si>
+  <si>
+    <t>GUI a schermo intero</t>
+  </si>
+  <si>
+    <t>File di Stato</t>
+  </si>
+  <si>
+    <t>Stato di carico...</t>
+  </si>
+  <si>
+    <t>Salva lo stato...</t>
+  </si>
+  <si>
+    <t>LED della tastiera</t>
+  </si>
+  <si>
+    <t>Modalità USB</t>
+  </si>
+  <si>
+    <t>Path:</t>
+  </si>
+  <si>
+    <t>Hardfile Settings</t>
+  </si>
+  <si>
+    <t>Geometry:</t>
+  </si>
+  <si>
+    <t>FileSys:</t>
+  </si>
+  <si>
+    <t>Device:</t>
+  </si>
+  <si>
+    <t>Boot priority:</t>
+  </si>
+  <si>
+    <t>Manual geometry</t>
+  </si>
+  <si>
+    <t>Read/write</t>
+  </si>
+  <si>
+    <t>Bootable</t>
+  </si>
+  <si>
+    <t>Do not mount</t>
+  </si>
+  <si>
+    <t>Global filesystem</t>
+  </si>
+  <si>
+    <t>HD Controller:</t>
+  </si>
+  <si>
+    <t>Full drive/RDB mode</t>
+  </si>
+  <si>
+    <t>Surfaces:</t>
+  </si>
+  <si>
+    <t>Sectors:</t>
+  </si>
+  <si>
+    <t>Cylinders:</t>
+  </si>
+  <si>
+    <t>Block size:</t>
+  </si>
+  <si>
+    <t>New hard disk image file</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>DOS type</t>
+  </si>
+  <si>
+    <t>Sparse file</t>
+  </si>
+  <si>
+    <t>Dynamic HDF</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Impostazioni del file rigido</t>
+  </si>
+  <si>
+    <t>Percorso:</t>
+  </si>
+  <si>
+    <t>Geometria:</t>
+  </si>
+  <si>
+    <t>Dispositivo:</t>
+  </si>
+  <si>
+    <t>Priorità di avvio:</t>
+  </si>
+  <si>
+    <t>Geometria manuale</t>
+  </si>
+  <si>
+    <t>Lettura/scrittura</t>
+  </si>
+  <si>
+    <t>Avviabile</t>
+  </si>
+  <si>
+    <t>Non montare</t>
+  </si>
+  <si>
+    <t>File system globale</t>
+  </si>
+  <si>
+    <t>Controllore HD:</t>
+  </si>
+  <si>
+    <t>Modalità full drive/RDB</t>
+  </si>
+  <si>
+    <t>Superfici:</t>
+  </si>
+  <si>
+    <t>Settori:</t>
+  </si>
+  <si>
+    <t>Cilindri:</t>
+  </si>
+  <si>
+    <t>Dim blocco:</t>
+  </si>
+  <si>
+    <t>Nuovo file immagine del disco rigido</t>
+  </si>
+  <si>
+    <t>Creare</t>
+  </si>
+  <si>
+    <t>Tipo DOS</t>
+  </si>
+  <si>
+    <t>File sparso</t>
+  </si>
+  <si>
+    <t>HDF dinamico</t>
+  </si>
+  <si>
+    <t>Annullamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2757,6 +2985,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2779,7 +3013,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2788,6 +3022,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3103,10 +3338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F497"/>
+  <dimension ref="A1:F538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
-      <selection activeCell="A498" sqref="A498"/>
+    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
+      <selection activeCell="C538" sqref="C538"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8085,7 +8320,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
         <v>830</v>
       </c>
@@ -8093,7 +8328,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
         <v>831</v>
       </c>
@@ -8101,7 +8336,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
         <v>832</v>
       </c>
@@ -8109,7 +8344,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
         <v>833</v>
       </c>
@@ -8117,7 +8352,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
         <v>834</v>
       </c>
@@ -8125,7 +8360,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
         <v>835</v>
       </c>
@@ -8133,7 +8368,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
         <v>836</v>
       </c>
@@ -8141,7 +8376,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
         <v>837</v>
       </c>
@@ -8149,7 +8384,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
         <v>838</v>
       </c>
@@ -8157,7 +8392,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
         <v>839</v>
       </c>
@@ -8165,28 +8400,25 @@
         <v>839</v>
       </c>
     </row>
-    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>135</v>
       </c>
       <c r="B475" t="s">
         <v>858</v>
       </c>
-      <c r="D475" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B476" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B477" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>138</v>
       </c>
@@ -8197,7 +8429,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
         <v>881</v>
       </c>
@@ -8205,7 +8437,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
         <v>882</v>
       </c>
@@ -8344,18 +8576,352 @@
         <v>894</v>
       </c>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>141</v>
       </c>
       <c r="B497" t="s">
         <v>774</v>
+      </c>
+    </row>
+    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B498" t="s">
+        <v>895</v>
+      </c>
+      <c r="C498" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B499" t="s">
+        <v>896</v>
+      </c>
+      <c r="C499" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B500" t="s">
+        <v>897</v>
+      </c>
+      <c r="C500" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B501" t="s">
+        <v>898</v>
+      </c>
+      <c r="C501" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B502" t="s">
+        <v>899</v>
+      </c>
+      <c r="C502" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B503" t="s">
+        <v>900</v>
+      </c>
+      <c r="C503" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="504" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B504" t="s">
+        <v>901</v>
+      </c>
+      <c r="C504" s="6" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B505" t="s">
+        <v>902</v>
+      </c>
+      <c r="C505" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B506" t="s">
+        <v>903</v>
+      </c>
+      <c r="C506" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B507" t="s">
+        <v>904</v>
+      </c>
+      <c r="C507" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B508" t="s">
+        <v>905</v>
+      </c>
+      <c r="C508" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B509" t="s">
+        <v>906</v>
+      </c>
+      <c r="C509" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B510" t="s">
+        <v>907</v>
+      </c>
+      <c r="C510" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B511" t="s">
+        <v>908</v>
+      </c>
+      <c r="C511" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B512" t="s">
+        <v>909</v>
+      </c>
+      <c r="C512" t="s">
+        <v>923</v>
+      </c>
+      <c r="D512" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>142</v>
+      </c>
+      <c r="B513" t="s">
+        <v>925</v>
+      </c>
+      <c r="C513" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B514" t="s">
+        <v>252</v>
+      </c>
+      <c r="C514" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B515" t="s">
+        <v>924</v>
+      </c>
+      <c r="C515" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B516" t="s">
+        <v>926</v>
+      </c>
+      <c r="C516" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B517" t="s">
+        <v>927</v>
+      </c>
+      <c r="C517" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B518" t="s">
+        <v>928</v>
+      </c>
+      <c r="C518" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B519" t="s">
+        <v>929</v>
+      </c>
+      <c r="C519" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B520" t="s">
+        <v>930</v>
+      </c>
+      <c r="C520" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B521" t="s">
+        <v>931</v>
+      </c>
+      <c r="C521" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B522" t="s">
+        <v>932</v>
+      </c>
+      <c r="C522" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B523" t="s">
+        <v>933</v>
+      </c>
+      <c r="C523" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B524" t="s">
+        <v>934</v>
+      </c>
+      <c r="C524" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B525" t="s">
+        <v>935</v>
+      </c>
+      <c r="C525" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B526" t="s">
+        <v>936</v>
+      </c>
+      <c r="C526" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B527" t="s">
+        <v>937</v>
+      </c>
+      <c r="C527" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B528" t="s">
+        <v>938</v>
+      </c>
+      <c r="C528" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="529" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B529" t="s">
+        <v>939</v>
+      </c>
+      <c r="C529" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="530" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B530" t="s">
+        <v>940</v>
+      </c>
+      <c r="C530" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="531" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B531" t="s">
+        <v>941</v>
+      </c>
+      <c r="C531" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="532" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B532" t="s">
+        <v>942</v>
+      </c>
+      <c r="C532" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="533" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B533" t="s">
+        <v>943</v>
+      </c>
+      <c r="C533" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="534" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B534" t="s">
+        <v>944</v>
+      </c>
+      <c r="C534" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="535" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B535" t="s">
+        <v>945</v>
+      </c>
+      <c r="C535" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="536" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B536" t="s">
+        <v>946</v>
+      </c>
+      <c r="C536" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="537" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B537" t="s">
+        <v>947</v>
+      </c>
+      <c r="C537" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="538" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B538" t="s">
+        <v>948</v>
+      </c>
+      <c r="C538" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D475" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D512" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Priorities and additional info translated
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB194F-825B-40DB-86AB-F0680CB5DBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D7A07-8FDD-4BB5-A737-17DC92D95F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="1860" windowWidth="27060" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="12345" yWindow="2700" windowWidth="27060" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="1041">
   <si>
     <t>ID</t>
   </si>
@@ -2948,6 +2948,216 @@
   </si>
   <si>
     <t>Annullamento</t>
+  </si>
+  <si>
+    <t>Volume Settings</t>
+  </si>
+  <si>
+    <t>Device name:</t>
+  </si>
+  <si>
+    <t>Select Directory</t>
+  </si>
+  <si>
+    <t>Select Archive or Plain File</t>
+  </si>
+  <si>
+    <t>Impostazioni del volume</t>
+  </si>
+  <si>
+    <t>Nome del dispositivo:</t>
+  </si>
+  <si>
+    <t>Volume label:</t>
+  </si>
+  <si>
+    <t>Etichetta del volume:</t>
+  </si>
+  <si>
+    <t>Selezionare la directory</t>
+  </si>
+  <si>
+    <t>Selezionare Archivio o File semplice</t>
+  </si>
+  <si>
+    <t>When Active</t>
+  </si>
+  <si>
+    <t>Run at priority:</t>
+  </si>
+  <si>
+    <t>Mouse uncaptured:</t>
+  </si>
+  <si>
+    <t>Pause emulation</t>
+  </si>
+  <si>
+    <t>Disable sound</t>
+  </si>
+  <si>
+    <t>When Inactive</t>
+  </si>
+  <si>
+    <t>Disable game controllers</t>
+  </si>
+  <si>
+    <t>When Minimized</t>
+  </si>
+  <si>
+    <t>File Extension Associations</t>
+  </si>
+  <si>
+    <t>Associate all</t>
+  </si>
+  <si>
+    <t>Deassociate all</t>
+  </si>
+  <si>
+    <t>Quando è attivo</t>
+  </si>
+  <si>
+    <t>Eseguire con priorità:</t>
+  </si>
+  <si>
+    <t>Topo non catturato:</t>
+  </si>
+  <si>
+    <t>Pausa emulazione</t>
+  </si>
+  <si>
+    <t>Disattivare il suono</t>
+  </si>
+  <si>
+    <t>Quando è inattivo</t>
+  </si>
+  <si>
+    <t>Disattivare i controller di gioco</t>
+  </si>
+  <si>
+    <t>Quando è ridotto al minimo</t>
+  </si>
+  <si>
+    <t>Associazioni di estensioni di file</t>
+  </si>
+  <si>
+    <t>Associare tutti</t>
+  </si>
+  <si>
+    <t>Dissociare tutti i</t>
+  </si>
+  <si>
+    <t>WinUAE Debugger</t>
+  </si>
+  <si>
+    <t>Debugger WinUAE</t>
+  </si>
+  <si>
+    <t>Additional Information Settings</t>
+  </si>
+  <si>
+    <t>Link:</t>
+  </si>
+  <si>
+    <t>Category:</t>
+  </si>
+  <si>
+    <t>Tags:</t>
+  </si>
+  <si>
+    <t>Ignore link</t>
+  </si>
+  <si>
+    <t>Autoload</t>
+  </si>
+  <si>
+    <t>Espulsione</t>
+  </si>
+  <si>
+    <t>Informazioni aggiuntive Impostazioni</t>
+  </si>
+  <si>
+    <t>Categoria:</t>
+  </si>
+  <si>
+    <t>Tag:</t>
+  </si>
+  <si>
+    <t>Ignorare il link</t>
+  </si>
+  <si>
+    <t>Carica automatica</t>
+  </si>
+  <si>
+    <t>OCS [] Original chipset. A1000 and most A500s.</t>
+  </si>
+  <si>
+    <t>ECS Agnus [] Enhanced chipset (ECS Agnus chip only). CDTV and later A500 and A2000 hardware revisions.</t>
+  </si>
+  <si>
+    <t>Full ECS [] Full ECS chipset (ECS Agnus and ECS Denise chips). A500+, A600 and A3000.</t>
+  </si>
+  <si>
+    <t>AGA [] Advanced Graphics Architecture chipset. A1200, A4000 and CD32.</t>
+  </si>
+  <si>
+    <t>ECS Denise [] Enhanced chipset (ECS Denise chip only). Normally paired with ECS Agnus.</t>
+  </si>
+  <si>
+    <t>NTSC [] North American and Japanese display standard, 60Hz refresh rate. Other countries use PAL (50Hz. display refresh rate)</t>
+  </si>
+  <si>
+    <t>Cycle-exact (Full) [] The most compatible A500/A1200 emulation mode.</t>
+  </si>
+  <si>
+    <t>Cycle-exact (DMA/Memory accesses)</t>
+  </si>
+  <si>
+    <t>Chipset Extra:</t>
+  </si>
+  <si>
+    <t>Keyboard connected</t>
+  </si>
+  <si>
+    <t>Subpixel display emulation</t>
+  </si>
+  <si>
+    <t>Immediate Blitter [] Faster but less compatible blitter emulation.</t>
+  </si>
+  <si>
+    <t>Wait for Blitter [] Compatibility hack for programs that don\'t wait for the blitter correctly, causing graphics corruption if CPU is too fast.</t>
+  </si>
+  <si>
+    <t>Video port display hardware:</t>
+  </si>
+  <si>
+    <t>Monitor:</t>
+  </si>
+  <si>
+    <t>Collision Level</t>
+  </si>
+  <si>
+    <t>None [] Collision hardware emulation disabled.</t>
+  </si>
+  <si>
+    <t>Sprites only [] Emulate only sprite vs. sprite collisions.</t>
+  </si>
+  <si>
+    <t>Sprites and Sprites vs. Playfield [] Recommended collision emulation level.</t>
+  </si>
+  <si>
+    <t>Full [] 100% collision hardware emulation. Only very few games need this option. Slowest.</t>
+  </si>
+  <si>
+    <t>Genlock</t>
+  </si>
+  <si>
+    <t>Genlock connected [] Allow boot sequence to detect genlock.</t>
+  </si>
+  <si>
+    <t>Include alpha channel in screenshots and video captures.</t>
+  </si>
+  <si>
+    <t>Keep aspect ratio</t>
   </si>
 </sst>
 </file>
@@ -3338,10 +3548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F538"/>
+  <dimension ref="A1:F597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A502" workbookViewId="0">
-      <selection activeCell="C538" sqref="C538"/>
+    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
+      <selection activeCell="B598" sqref="B598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8576,7 +8786,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="497" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>141</v>
       </c>
@@ -8584,7 +8794,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="498" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
         <v>895</v>
       </c>
@@ -8592,7 +8802,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="499" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
         <v>896</v>
       </c>
@@ -8600,7 +8810,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="500" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
         <v>897</v>
       </c>
@@ -8608,7 +8818,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="501" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B501" t="s">
         <v>898</v>
       </c>
@@ -8616,7 +8826,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="502" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B502" t="s">
         <v>899</v>
       </c>
@@ -8624,7 +8834,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="503" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B503" t="s">
         <v>900</v>
       </c>
@@ -8632,7 +8842,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="504" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B504" t="s">
         <v>901</v>
       </c>
@@ -8640,7 +8850,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="505" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B505" t="s">
         <v>902</v>
       </c>
@@ -8648,7 +8858,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="506" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B506" t="s">
         <v>903</v>
       </c>
@@ -8656,7 +8866,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="507" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B507" t="s">
         <v>904</v>
       </c>
@@ -8664,7 +8874,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B508" t="s">
         <v>905</v>
       </c>
@@ -8672,7 +8882,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B509" t="s">
         <v>906</v>
       </c>
@@ -8680,7 +8890,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B510" t="s">
         <v>907</v>
       </c>
@@ -8688,7 +8898,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B511" t="s">
         <v>908</v>
       </c>
@@ -8696,15 +8906,12 @@
         <v>922</v>
       </c>
     </row>
-    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B512" t="s">
         <v>909</v>
       </c>
       <c r="C512" t="s">
         <v>923</v>
-      </c>
-      <c r="D512" s="5" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
@@ -8838,7 +9045,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="529" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B529" t="s">
         <v>939</v>
       </c>
@@ -8846,7 +9053,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="530" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
         <v>940</v>
       </c>
@@ -8854,7 +9061,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="531" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
         <v>941</v>
       </c>
@@ -8862,7 +9069,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="532" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B532" t="s">
         <v>942</v>
       </c>
@@ -8870,7 +9077,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="533" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B533" t="s">
         <v>943</v>
       </c>
@@ -8878,7 +9085,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="534" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
         <v>944</v>
       </c>
@@ -8886,7 +9093,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="535" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B535" t="s">
         <v>945</v>
       </c>
@@ -8894,7 +9101,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="536" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B536" t="s">
         <v>946</v>
       </c>
@@ -8902,7 +9109,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="537" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B537" t="s">
         <v>947</v>
       </c>
@@ -8910,18 +9117,430 @@
         <v>947</v>
       </c>
     </row>
-    <row r="538" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B538" t="s">
         <v>948</v>
       </c>
       <c r="C538" t="s">
         <v>970</v>
+      </c>
+    </row>
+    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A539">
+        <v>143</v>
+      </c>
+      <c r="B539" t="s">
+        <v>971</v>
+      </c>
+      <c r="C539" t="s">
+        <v>975</v>
+      </c>
+      <c r="D539" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B540" t="s">
+        <v>972</v>
+      </c>
+      <c r="C540" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B541" t="s">
+        <v>977</v>
+      </c>
+      <c r="C541" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B542" t="s">
+        <v>924</v>
+      </c>
+      <c r="C542" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B543" t="s">
+        <v>931</v>
+      </c>
+      <c r="C543" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B544" t="s">
+        <v>932</v>
+      </c>
+      <c r="C544" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B545" t="s">
+        <v>929</v>
+      </c>
+      <c r="C545" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B546" t="s">
+        <v>973</v>
+      </c>
+      <c r="C546" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B547" t="s">
+        <v>974</v>
+      </c>
+      <c r="C547" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B548" t="s">
+        <v>947</v>
+      </c>
+      <c r="C548" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B549" t="s">
+        <v>948</v>
+      </c>
+      <c r="C549" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B550" t="s">
+        <v>688</v>
+      </c>
+      <c r="C550" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>144</v>
+      </c>
+      <c r="B551" t="s">
+        <v>981</v>
+      </c>
+      <c r="C551" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B552" t="s">
+        <v>982</v>
+      </c>
+      <c r="C552" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B553" t="s">
+        <v>983</v>
+      </c>
+      <c r="C553" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B554" t="s">
+        <v>984</v>
+      </c>
+      <c r="C554" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B555" t="s">
+        <v>985</v>
+      </c>
+      <c r="C555" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B556" t="s">
+        <v>986</v>
+      </c>
+      <c r="C556" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B557" t="s">
+        <v>987</v>
+      </c>
+      <c r="C557" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B558" t="s">
+        <v>988</v>
+      </c>
+      <c r="C558" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B559" t="s">
+        <v>989</v>
+      </c>
+      <c r="C559" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B560" t="s">
+        <v>990</v>
+      </c>
+      <c r="C560" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B561" t="s">
+        <v>991</v>
+      </c>
+      <c r="C561" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A562">
+        <v>152</v>
+      </c>
+      <c r="B562" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C562" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563">
+        <v>153</v>
+      </c>
+      <c r="B563" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C563" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B564" t="s">
+        <v>924</v>
+      </c>
+      <c r="C564" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B565" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C565" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B566" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C566" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B567" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C567" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B568" t="s">
+        <v>1009</v>
+      </c>
+      <c r="C568" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B569" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C569" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B570" t="s">
+        <v>947</v>
+      </c>
+      <c r="C570" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B571" t="s">
+        <v>948</v>
+      </c>
+      <c r="C571" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572">
+        <v>154</v>
+      </c>
+      <c r="B572" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B573" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B574" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B575" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B576" t="s">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="577" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B577" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="578" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B578" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="579" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B579" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="580" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B580" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="581" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B581" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="582" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B582" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="583" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B583" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="584" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B584" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="585" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B585" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="586" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B586" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="587" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B587" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="588" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B588" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="589" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B589" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="590" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B590" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="591" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B591" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="592" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B592" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B593" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="594" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B594" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="595" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B595" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="596" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B596" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="597" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B597" t="s">
+        <v>1040</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D512" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D539" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Chipset Advanced chipset translations
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5D7A07-8FDD-4BB5-A737-17DC92D95F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93395339-0CA3-4404-B048-0F12DBF595CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12345" yWindow="2700" windowWidth="27060" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="13725" yWindow="675" windowWidth="24660" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1098">
   <si>
     <t>ID</t>
   </si>
@@ -3158,6 +3158,177 @@
   </si>
   <si>
     <t>Keep aspect ratio</t>
+  </si>
+  <si>
+    <t>OCS [] Chipset originale. A1000 e la maggior parte degli A500.</t>
+  </si>
+  <si>
+    <t>ECS Agnus [] Chipset migliorato (solo chip ECS Agnus). CDTV e successive revisioni hardware A500 e A2000.</t>
+  </si>
+  <si>
+    <t>ECS completo [] Chipset ECS completo (chip ECS Agnus e ECS Denise). A500+, A600 e A3000.</t>
+  </si>
+  <si>
+    <t>AGA [] Chipset Advanced Graphics Architecture. A1200, A4000 e CD32.</t>
+  </si>
+  <si>
+    <t>ECS Denise [] Chipset avanzato (solo chip ECS Denise). Normalmente abbinato a ECS Agnus.</t>
+  </si>
+  <si>
+    <t>NTSC [] Standard di visualizzazione nordamericano e giapponese, frequenza di aggiornamento di 60Hz. Gli altri paesi utilizzano lo standard PAL (frequenza di aggiornamento a 50Hz).</t>
+  </si>
+  <si>
+    <t>Cycle-exact (Full) [] La modalità di emulazione A500/A1200 più compatibile.</t>
+  </si>
+  <si>
+    <t>Cycle-exact (accessi DMA/memoria)</t>
+  </si>
+  <si>
+    <t>Tastiera collegata</t>
+  </si>
+  <si>
+    <t>Emulazione del display subpixel</t>
+  </si>
+  <si>
+    <t>Immediate Blitter [] Emulazione di blitter più veloce ma meno compatibile.</t>
+  </si>
+  <si>
+    <t>Wait for Blitter [] Hack di compatibilità per i programmi che non attendono correttamente il blitter, causando la corruzione della grafica se la CPU è troppo veloce.</t>
+  </si>
+  <si>
+    <t>Hardware di visualizzazione della porta video:</t>
+  </si>
+  <si>
+    <t>Livello di collisione</t>
+  </si>
+  <si>
+    <t>Nessuna [] Emulazione hardware di collisione disabilitata.</t>
+  </si>
+  <si>
+    <t>Solo sprite [] Emula solo le collisioni tra sprite.</t>
+  </si>
+  <si>
+    <t>Sprites e Sprites vs. Playfield [] Livello di emulazione delle collisioni consigliato.</t>
+  </si>
+  <si>
+    <t>Emulazione hardware completa [] 100% collisione. Solo pochissimi giochi necessitano di questa opzione. Il più lento.</t>
+  </si>
+  <si>
+    <t>Genlock collegato [] Consente alla sequenza di avvio di rilevare il genlock.</t>
+  </si>
+  <si>
+    <t>Includere il canale alfa nelle schermate e nelle catture video.</t>
+  </si>
+  <si>
+    <t>Mantenere il rapporto d'aspetto</t>
+  </si>
+  <si>
+    <t>Compatible Settings</t>
+  </si>
+  <si>
+    <t>Battery Backed Up Real Time Clock</t>
+  </si>
+  <si>
+    <t>CIA-A TOD Clock Source</t>
+  </si>
+  <si>
+    <t>Vertical Sync</t>
+  </si>
+  <si>
+    <t>Power Supply 50Hz</t>
+  </si>
+  <si>
+    <t>Power Supply 60Hz</t>
+  </si>
+  <si>
+    <t>Chipset Features</t>
+  </si>
+  <si>
+    <t>Unmapped address space:</t>
+  </si>
+  <si>
+    <t>Internal SCSI Hardware</t>
+  </si>
+  <si>
+    <t>Chipset Revision</t>
+  </si>
+  <si>
+    <t>Ramsey revision:</t>
+  </si>
+  <si>
+    <t>Fat Gary revision:</t>
+  </si>
+  <si>
+    <t>Agnus/Alice revision:</t>
+  </si>
+  <si>
+    <t>Denise/Lisa revision:</t>
+  </si>
+  <si>
+    <t>Impostazioni compatibili</t>
+  </si>
+  <si>
+    <t>Orologio in tempo reale a batteria</t>
+  </si>
+  <si>
+    <t>CIA-A Sorgente di clock TOD</t>
+  </si>
+  <si>
+    <t>Sincronizzazione vert</t>
+  </si>
+  <si>
+    <t>Alimentazione 50Hz</t>
+  </si>
+  <si>
+    <t>Alimentazione 60Hz</t>
+  </si>
+  <si>
+    <t>Caratteristiche del chipset</t>
+  </si>
+  <si>
+    <t>Spazio indirizzi non mappato:</t>
+  </si>
+  <si>
+    <t>Hardware SCSI interno</t>
+  </si>
+  <si>
+    <t>Revisione del chipset</t>
+  </si>
+  <si>
+    <t>Revisione Ramsey:</t>
+  </si>
+  <si>
+    <t>Revisione Fat Gary:</t>
+  </si>
+  <si>
+    <t>Revisione Agnus/Alice:</t>
+  </si>
+  <si>
+    <t>Revisione Denise/Lisa:</t>
+  </si>
+  <si>
+    <t>Composite color burst</t>
+  </si>
+  <si>
+    <t>Raffica di colori compositi</t>
+  </si>
+  <si>
+    <t>Custom register byte write bug</t>
+  </si>
+  <si>
+    <t>Bug di scrittura dei byte del registro personalizzato</t>
+  </si>
+  <si>
+    <t>KS ROM has Chip RAM speed</t>
+  </si>
+  <si>
+    <t>KS ROM ha la velocità di Chip RAM</t>
+  </si>
+  <si>
+    <t>CIA 391078-01 [] CIA revision that can\'t read IO pin status in output mode</t>
+  </si>
+  <si>
+    <t>CIA 391078-01 [] Revisione CIA che non può leggere lo stato del pin IO in modalità di uscita</t>
   </si>
 </sst>
 </file>
@@ -3548,10 +3719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F597"/>
+  <dimension ref="A1:F616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A545" workbookViewId="0">
-      <selection activeCell="B598" sqref="B598"/>
+    <sheetView tabSelected="1" topLeftCell="A573" workbookViewId="0">
+      <selection activeCell="B612" sqref="B612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9045,7 +9216,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B529" t="s">
         <v>939</v>
       </c>
@@ -9053,7 +9224,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B530" t="s">
         <v>940</v>
       </c>
@@ -9061,7 +9232,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B531" t="s">
         <v>941</v>
       </c>
@@ -9069,7 +9240,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B532" t="s">
         <v>942</v>
       </c>
@@ -9077,7 +9248,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B533" t="s">
         <v>943</v>
       </c>
@@ -9085,7 +9256,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B534" t="s">
         <v>944</v>
       </c>
@@ -9093,7 +9264,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B535" t="s">
         <v>945</v>
       </c>
@@ -9101,7 +9272,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B536" t="s">
         <v>946</v>
       </c>
@@ -9109,7 +9280,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B537" t="s">
         <v>947</v>
       </c>
@@ -9117,7 +9288,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B538" t="s">
         <v>948</v>
       </c>
@@ -9125,7 +9296,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A539">
         <v>143</v>
       </c>
@@ -9135,11 +9306,8 @@
       <c r="C539" t="s">
         <v>975</v>
       </c>
-      <c r="D539" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="540" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B540" t="s">
         <v>972</v>
       </c>
@@ -9147,7 +9315,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B541" t="s">
         <v>977</v>
       </c>
@@ -9155,7 +9323,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B542" t="s">
         <v>924</v>
       </c>
@@ -9163,7 +9331,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B543" t="s">
         <v>931</v>
       </c>
@@ -9171,7 +9339,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B544" t="s">
         <v>932</v>
       </c>
@@ -9411,136 +9579,372 @@
       <c r="B572" t="s">
         <v>17</v>
       </c>
+      <c r="C572" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B573" t="s">
         <v>1017</v>
       </c>
+      <c r="C573" t="s">
+        <v>1041</v>
+      </c>
     </row>
     <row r="574" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B574" t="s">
         <v>1018</v>
       </c>
+      <c r="C574" t="s">
+        <v>1042</v>
+      </c>
     </row>
     <row r="575" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B575" t="s">
         <v>1019</v>
       </c>
+      <c r="C575" t="s">
+        <v>1043</v>
+      </c>
     </row>
     <row r="576" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B576" t="s">
         <v>1020</v>
       </c>
-    </row>
-    <row r="577" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C576" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="577" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B577" t="s">
         <v>1021</v>
       </c>
-    </row>
-    <row r="578" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C577" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="578" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B578" t="s">
         <v>1022</v>
       </c>
-    </row>
-    <row r="579" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C578" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="579" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B579" t="s">
         <v>1023</v>
       </c>
-    </row>
-    <row r="580" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C579" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="580" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B580" t="s">
         <v>1024</v>
       </c>
-    </row>
-    <row r="581" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C580" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="581" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B581" t="s">
         <v>1025</v>
       </c>
-    </row>
-    <row r="582" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C581" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="582" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B582" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="583" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C582" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="583" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B583" t="s">
         <v>1026</v>
       </c>
-    </row>
-    <row r="584" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C583" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="584" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B584" t="s">
         <v>1027</v>
       </c>
-    </row>
-    <row r="585" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C584" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="585" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B585" t="s">
         <v>1028</v>
       </c>
-    </row>
-    <row r="586" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C585" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="586" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B586" t="s">
         <v>1029</v>
       </c>
-    </row>
-    <row r="587" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C586" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="587" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B587" t="s">
         <v>1030</v>
       </c>
-    </row>
-    <row r="588" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C587" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="588" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B588" t="s">
         <v>1031</v>
       </c>
-    </row>
-    <row r="589" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C588" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="589" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B589" t="s">
         <v>1032</v>
       </c>
-    </row>
-    <row r="590" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C589" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="590" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B590" t="s">
         <v>1033</v>
       </c>
-    </row>
-    <row r="591" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C590" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="591" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B591" t="s">
         <v>1034</v>
       </c>
-    </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C591" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="592" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B592" t="s">
         <v>1035</v>
       </c>
-    </row>
-    <row r="593" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C592" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="593" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B593" t="s">
         <v>1036</v>
       </c>
-    </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C593" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="594" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B594" t="s">
         <v>1037</v>
       </c>
-    </row>
-    <row r="595" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C594" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="595" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B595" t="s">
         <v>1038</v>
       </c>
-    </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C595" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="596" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B596" t="s">
         <v>1039</v>
       </c>
-    </row>
-    <row r="597" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C596" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="597" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B597" t="s">
         <v>1040</v>
+      </c>
+      <c r="C597" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E597" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="598" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A598">
+        <v>155</v>
+      </c>
+      <c r="B598" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C598" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="599" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B599" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C599" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="600" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B600" t="s">
+        <v>721</v>
+      </c>
+      <c r="C600" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="601" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B601" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C601" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="602" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B602" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C602" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="603" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B603" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C603" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="604" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B604" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C604" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="605" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B605" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C605" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="606" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B606" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C606" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="607" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B607" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C607" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="608" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B608" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C608" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="609" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B609" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C609" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="610" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B610" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C610" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="611" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B611" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C611" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="612" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B612" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C612" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="613" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B613" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C613" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="614" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B614" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C614" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="615" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B615" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C615" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="616" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B616" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C616" t="s">
+        <v>1089</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D539" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="E597" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Output and filter translations added
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93395339-0CA3-4404-B048-0F12DBF595CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA51CCB-0830-4E81-8434-1D674B85BF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13725" yWindow="675" windowWidth="24660" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="8205" yWindow="945" windowWidth="24660" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="1098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="1162">
   <si>
     <t>ID</t>
   </si>
@@ -3329,6 +3329,198 @@
   </si>
   <si>
     <t>CIA 391078-01 [] Revisione CIA che non può leggere lo stato del pin IO in modalità di uscita</t>
+  </si>
+  <si>
+    <t>Output Properties</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Disable frame rate limit</t>
+  </si>
+  <si>
+    <t>Disable sound output</t>
+  </si>
+  <si>
+    <t>Capture before filtering</t>
+  </si>
+  <si>
+    <t>Disable sound sync</t>
+  </si>
+  <si>
+    <t>AVI output enabled</t>
+  </si>
+  <si>
+    <t>Ripper</t>
+  </si>
+  <si>
+    <t>Save screenshot</t>
+  </si>
+  <si>
+    <t>Pro Wizard 1.62</t>
+  </si>
+  <si>
+    <t>Sample ripper</t>
+  </si>
+  <si>
+    <t>Take screenshot before filtering</t>
+  </si>
+  <si>
+    <t>Autoclip screenshot</t>
+  </si>
+  <si>
+    <t>Re-recorder</t>
+  </si>
+  <si>
+    <t>Play recording</t>
+  </si>
+  <si>
+    <t>Automatic replay</t>
+  </si>
+  <si>
+    <t>Recording rate (seconds):</t>
+  </si>
+  <si>
+    <t>Re-recording enabled</t>
+  </si>
+  <si>
+    <t>Save recording</t>
+  </si>
+  <si>
+    <t>Recording buffers:</t>
+  </si>
+  <si>
+    <t>Proprietà di uscita</t>
+  </si>
+  <si>
+    <t>Disattivare il limite della frequenza dei fotogrammi</t>
+  </si>
+  <si>
+    <t>Disattivare l'uscita audio</t>
+  </si>
+  <si>
+    <t>Cattura prima del filtraggio</t>
+  </si>
+  <si>
+    <t>Disattivare la sincronizzazione del suono</t>
+  </si>
+  <si>
+    <t>Uscita AVI abilitata</t>
+  </si>
+  <si>
+    <t>Squartatore</t>
+  </si>
+  <si>
+    <t>Salva screenshot</t>
+  </si>
+  <si>
+    <t>Ripper campione</t>
+  </si>
+  <si>
+    <t>Scattare un'istantanea prima del filtraggio</t>
+  </si>
+  <si>
+    <t>Schermata Autoclip</t>
+  </si>
+  <si>
+    <t>Ri-registratore</t>
+  </si>
+  <si>
+    <t>Riproduzione della registrazione</t>
+  </si>
+  <si>
+    <t>Velocità di registrazione (secondi):</t>
+  </si>
+  <si>
+    <t>Riproduzione automatica</t>
+  </si>
+  <si>
+    <t>Registrazione abilitata</t>
+  </si>
+  <si>
+    <t>Salvare la registrazione</t>
+  </si>
+  <si>
+    <t>Buffer di registrazione:</t>
+  </si>
+  <si>
+    <t>Filter Settings</t>
+  </si>
+  <si>
+    <t>Horiz. size:</t>
+  </si>
+  <si>
+    <t>Vert. size:</t>
+  </si>
+  <si>
+    <t>Horiz. position:</t>
+  </si>
+  <si>
+    <t>Vert. position:</t>
+  </si>
+  <si>
+    <t>Aspect Ratio Correction</t>
+  </si>
+  <si>
+    <t>Keep autoscale aspect</t>
+  </si>
+  <si>
+    <t>Extra Settings</t>
+  </si>
+  <si>
+    <t>Presets</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Impostazioni del filtro</t>
+  </si>
+  <si>
+    <t>Ripristino delle impostazioni predefinite</t>
+  </si>
+  <si>
+    <t>Dimensione orizzontale:</t>
+  </si>
+  <si>
+    <t>Dimensione Vert:</t>
+  </si>
+  <si>
+    <t>Posizione orizzontale:</t>
+  </si>
+  <si>
+    <t>Posizione verticale:</t>
+  </si>
+  <si>
+    <t>Correzione del rapporto d'aspetto</t>
+  </si>
+  <si>
+    <t>Mantenere l'aspetto di autoscala</t>
+  </si>
+  <si>
+    <t>Impostazioni extra</t>
+  </si>
+  <si>
+    <t>Preimpostazioni</t>
+  </si>
+  <si>
+    <t>Caricare</t>
+  </si>
+  <si>
+    <t>Salvare</t>
+  </si>
+  <si>
+    <t>Cancellare</t>
   </si>
 </sst>
 </file>
@@ -3719,10 +3911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F616"/>
+  <dimension ref="A1:F652"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A573" workbookViewId="0">
-      <selection activeCell="B612" sqref="B612"/>
+    <sheetView tabSelected="1" topLeftCell="A624" workbookViewId="0">
+      <selection activeCell="A653" sqref="A653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9877,7 +10069,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="609" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B609" t="s">
         <v>1094</v>
       </c>
@@ -9885,7 +10077,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="610" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B610" t="s">
         <v>1096</v>
       </c>
@@ -9893,7 +10085,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="611" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B611" t="s">
         <v>1070</v>
       </c>
@@ -9901,7 +10093,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="612" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B612" t="s">
         <v>1071</v>
       </c>
@@ -9909,7 +10101,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="613" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B613" t="s">
         <v>1072</v>
       </c>
@@ -9917,7 +10109,7 @@
         <v>1086</v>
       </c>
     </row>
-    <row r="614" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B614" t="s">
         <v>1073</v>
       </c>
@@ -9925,7 +10117,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="615" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B615" t="s">
         <v>1074</v>
       </c>
@@ -9933,12 +10125,303 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="616" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B616" t="s">
         <v>1075</v>
       </c>
       <c r="C616" t="s">
         <v>1089</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A617">
+        <v>157</v>
+      </c>
+      <c r="B617" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C617" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B618" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C618" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B619" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C619" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B620" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C620" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B621" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C621" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B622" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C622" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B623" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C623" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B624" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C624" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B625" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C625" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B626" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C626" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B627" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C627" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B628" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C628" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B629" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C629" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B630" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C630" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B631" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C631" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B632" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C632" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B633" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C633" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B634" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C634" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B635" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C635" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B636" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C636" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B637" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C637" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A638">
+        <v>160</v>
+      </c>
+      <c r="B638" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C638" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B639" t="s">
+        <v>624</v>
+      </c>
+      <c r="C639" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B640" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C640" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B641" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C641" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B642" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C642" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B643" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C643" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B644" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C644" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B645" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C645" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B646" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C646" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B647" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C647" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B648" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C648" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B649" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C649" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B650" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C650" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B651" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C651" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A652">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hard disk, input and floppy drive translations
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA51CCB-0830-4E81-8434-1D674B85BF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9077A249-DF7F-4DB1-8991-3D6ABC4BD588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8205" yWindow="945" windowWidth="24660" windowHeight="15615" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="17145" yWindow="2955" windowWidth="21255" windowHeight="15315" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="1162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1201">
   <si>
     <t>ID</t>
   </si>
@@ -3521,6 +3521,123 @@
   </si>
   <si>
     <t>Cancellare</t>
+  </si>
+  <si>
+    <t>Harddrive Settings</t>
+  </si>
+  <si>
+    <t>Hard drive:</t>
+  </si>
+  <si>
+    <t>Create hard disk image file</t>
+  </si>
+  <si>
+    <t>Read Identity</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Add hard drive</t>
+  </si>
+  <si>
+    <t>Test [] Test input mappings.</t>
+  </si>
+  <si>
+    <t>Remap [] Find and remap quickly.</t>
+  </si>
+  <si>
+    <t>Joystick dead zone (%):</t>
+  </si>
+  <si>
+    <t>Autofire rate (lines):</t>
+  </si>
+  <si>
+    <t>Digital joy-mouse speed:</t>
+  </si>
+  <si>
+    <t>Analog joy-mouse speed:</t>
+  </si>
+  <si>
+    <t>Copy from:</t>
+  </si>
+  <si>
+    <t>Swap 1&lt;&gt;2</t>
+  </si>
+  <si>
+    <t>Device enabled</t>
+  </si>
+  <si>
+    <t>Impostazioni del disco rigido</t>
+  </si>
+  <si>
+    <t>Disco rigido:</t>
+  </si>
+  <si>
+    <t>Creare un file immagine del disco rigido</t>
+  </si>
+  <si>
+    <t>Leggi Identità</t>
+  </si>
+  <si>
+    <t>Blocco</t>
+  </si>
+  <si>
+    <t>Identità</t>
+  </si>
+  <si>
+    <t>Dim del blocco:</t>
+  </si>
+  <si>
+    <t>Aggiungere un disco rigido</t>
+  </si>
+  <si>
+    <t>Dispositivo abilitato</t>
+  </si>
+  <si>
+    <t>Test [] Prova le mappature degli ingressi.</t>
+  </si>
+  <si>
+    <t>Remap [] Trova e rimappa rapidamente.</t>
+  </si>
+  <si>
+    <t>Zona morta del joystick (%):</t>
+  </si>
+  <si>
+    <t>Velocità di fuoco automatico (linee):</t>
+  </si>
+  <si>
+    <t>Velocità del joy-mouse digitale:</t>
+  </si>
+  <si>
+    <t>Velocità del joy-mouse analogico:</t>
+  </si>
+  <si>
+    <t>Copia da:</t>
+  </si>
+  <si>
+    <t>Scambio 1&lt;&gt;2</t>
+  </si>
+  <si>
+    <t>Insert floppy disk image</t>
+  </si>
+  <si>
+    <t>Remove floppy disk image</t>
+  </si>
+  <si>
+    <t>Remove all</t>
+  </si>
+  <si>
+    <t>Inserire l'immagine del dischetto</t>
+  </si>
+  <si>
+    <t>Rimuovere l'immagine del dischetto</t>
+  </si>
+  <si>
+    <t>Rimuovi tutto</t>
   </si>
 </sst>
 </file>
@@ -3911,10 +4028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F652"/>
+  <dimension ref="A1:F681"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A624" workbookViewId="0">
-      <selection activeCell="A653" sqref="A653"/>
+    <sheetView tabSelected="1" topLeftCell="A648" workbookViewId="0">
+      <selection activeCell="A682" sqref="A682"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9935,7 +10052,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="593" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B593" t="s">
         <v>1036</v>
       </c>
@@ -9943,7 +10060,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="594" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B594" t="s">
         <v>1037</v>
       </c>
@@ -9951,7 +10068,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="595" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B595" t="s">
         <v>1038</v>
       </c>
@@ -9959,7 +10076,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="596" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B596" t="s">
         <v>1039</v>
       </c>
@@ -9967,18 +10084,15 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="597" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B597" t="s">
         <v>1040</v>
       </c>
       <c r="C597" t="s">
         <v>1061</v>
       </c>
-      <c r="E597" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="598" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A598">
         <v>155</v>
       </c>
@@ -9989,7 +10103,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="599" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B599" t="s">
         <v>1063</v>
       </c>
@@ -9997,7 +10111,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="600" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B600" t="s">
         <v>721</v>
       </c>
@@ -10005,7 +10119,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="601" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B601" t="s">
         <v>1064</v>
       </c>
@@ -10013,7 +10127,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="602" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B602" t="s">
         <v>1065</v>
       </c>
@@ -10021,7 +10135,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="603" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B603" t="s">
         <v>1066</v>
       </c>
@@ -10029,7 +10143,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="604" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B604" t="s">
         <v>1067</v>
       </c>
@@ -10037,7 +10151,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="605" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B605" t="s">
         <v>1068</v>
       </c>
@@ -10045,7 +10159,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="606" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B606" t="s">
         <v>1069</v>
       </c>
@@ -10053,7 +10167,7 @@
         <v>1083</v>
       </c>
     </row>
-    <row r="607" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B607" t="s">
         <v>1090</v>
       </c>
@@ -10061,7 +10175,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="608" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B608" t="s">
         <v>1092</v>
       </c>
@@ -10331,7 +10445,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B641" t="s">
         <v>1139</v>
       </c>
@@ -10339,7 +10453,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B642" t="s">
         <v>1140</v>
       </c>
@@ -10347,7 +10461,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B643" t="s">
         <v>1141</v>
       </c>
@@ -10355,7 +10469,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B644" t="s">
         <v>1142</v>
       </c>
@@ -10363,7 +10477,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B645" t="s">
         <v>1143</v>
       </c>
@@ -10371,7 +10485,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B646" t="s">
         <v>1040</v>
       </c>
@@ -10379,7 +10493,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B647" t="s">
         <v>1144</v>
       </c>
@@ -10387,7 +10501,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B648" t="s">
         <v>1145</v>
       </c>
@@ -10395,7 +10509,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B649" t="s">
         <v>1148</v>
       </c>
@@ -10403,7 +10517,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B650" t="s">
         <v>1146</v>
       </c>
@@ -10411,7 +10525,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B651" t="s">
         <v>1147</v>
       </c>
@@ -10419,15 +10533,259 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>163</v>
+      </c>
+      <c r="B652" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C652" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D652" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="653" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B653" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C653" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="654" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B654" t="s">
+        <v>926</v>
+      </c>
+      <c r="C654" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B655" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C655" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B656" t="s">
+        <v>931</v>
+      </c>
+      <c r="C656" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B657" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C657" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B658" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C658" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B659" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C659" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B660" t="s">
+        <v>930</v>
+      </c>
+      <c r="C660" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B661" t="s">
+        <v>937</v>
+      </c>
+      <c r="C661" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B662" t="s">
+        <v>938</v>
+      </c>
+      <c r="C662" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B663" t="s">
+        <v>939</v>
+      </c>
+      <c r="C663" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B664" t="s">
+        <v>940</v>
+      </c>
+      <c r="C664" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B665" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C665" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B666" t="s">
+        <v>948</v>
+      </c>
+      <c r="C666" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A667">
+        <v>171</v>
+      </c>
+      <c r="B667" t="s">
+        <v>773</v>
+      </c>
+      <c r="C667" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B668" t="s">
+        <v>774</v>
+      </c>
+      <c r="C668" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B669" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C669" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B670" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C670" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B671" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C671" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B672" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C672" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B673" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C673" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B674" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C674" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B675" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C675" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B676" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C676" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B677" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C677" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A678">
+        <v>172</v>
+      </c>
+      <c r="B678" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C678" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B679" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C679" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B680" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C680" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A681">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="E597" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D652" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Paths and Quickstart translations
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9077A249-DF7F-4DB1-8991-3D6ABC4BD588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8E3666-B037-47D9-8EE3-950850393DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17145" yWindow="2955" windowWidth="21255" windowHeight="15315" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="14235" yWindow="2205" windowWidth="23925" windowHeight="15315" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1276">
   <si>
     <t>ID</t>
   </si>
@@ -3638,6 +3638,231 @@
   </si>
   <si>
     <t>Rimuovi tutto</t>
+  </si>
+  <si>
+    <t>System ROMs:</t>
+  </si>
+  <si>
+    <t>Scan subfolders</t>
+  </si>
+  <si>
+    <t>Configuration files:</t>
+  </si>
+  <si>
+    <t>Cache Configuration files</t>
+  </si>
+  <si>
+    <t>Cache Boxart files</t>
+  </si>
+  <si>
+    <t>Screenshots:</t>
+  </si>
+  <si>
+    <t>State files:</t>
+  </si>
+  <si>
+    <t>Videos:</t>
+  </si>
+  <si>
+    <t>Saveimages:</t>
+  </si>
+  <si>
+    <t>Use original image\'s path</t>
+  </si>
+  <si>
+    <t>Rips:</t>
+  </si>
+  <si>
+    <t>Clear registry</t>
+  </si>
+  <si>
+    <t>Rescan ROMs</t>
+  </si>
+  <si>
+    <t>Clear disk history</t>
+  </si>
+  <si>
+    <t>Use relative paths</t>
+  </si>
+  <si>
+    <t>Portable mode</t>
+  </si>
+  <si>
+    <t>Debug logging</t>
+  </si>
+  <si>
+    <t>Enable full logging</t>
+  </si>
+  <si>
+    <t>Log window</t>
+  </si>
+  <si>
+    <t>Save All [] Create zip file that includes both logs and config file.</t>
+  </si>
+  <si>
+    <t>Open [] Open selected file.</t>
+  </si>
+  <si>
+    <t>ROM di sistema:</t>
+  </si>
+  <si>
+    <t>Scansione di sottocartelle</t>
+  </si>
+  <si>
+    <t>File di configurazione:</t>
+  </si>
+  <si>
+    <t>File di configurazione della cache</t>
+  </si>
+  <si>
+    <t>Cache dei file Boxart</t>
+  </si>
+  <si>
+    <t>Screenshot:</t>
+  </si>
+  <si>
+    <t>Fascicoli di Stato:</t>
+  </si>
+  <si>
+    <t>Video:</t>
+  </si>
+  <si>
+    <t>Salva immagini:</t>
+  </si>
+  <si>
+    <t>Utilizzare il percorso dell'immagine originale</t>
+  </si>
+  <si>
+    <t>Strappi:</t>
+  </si>
+  <si>
+    <t>Reset [] Ripristino delle impostazioni predefinite</t>
+  </si>
+  <si>
+    <t>Cancella il registro</t>
+  </si>
+  <si>
+    <t>Rescan delle ROM</t>
+  </si>
+  <si>
+    <t>Cancella la cronologia del disco</t>
+  </si>
+  <si>
+    <t>Utilizzare percorsi relativi</t>
+  </si>
+  <si>
+    <t>Modalità portatile</t>
+  </si>
+  <si>
+    <t>Registrazione di debug</t>
+  </si>
+  <si>
+    <t>Abilita la registrazione completa</t>
+  </si>
+  <si>
+    <t>Finestra del registro</t>
+  </si>
+  <si>
+    <t>Salva tutto [] Crea un file zip che include sia i log che il file di configurazione.</t>
+  </si>
+  <si>
+    <t>Apri [] Aprire il file selezionato.</t>
+  </si>
+  <si>
+    <t>Emulated Hardware</t>
+  </si>
+  <si>
+    <t>Model:</t>
+  </si>
+  <si>
+    <t>Configuration:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compatibility vs Required CPU Power </t>
+  </si>
+  <si>
+    <t>Best compatibility</t>
+  </si>
+  <si>
+    <t>Low compatibility</t>
+  </si>
+  <si>
+    <t>Host Configuration</t>
+  </si>
+  <si>
+    <t>Emulated Drives</t>
+  </si>
+  <si>
+    <t>Floppy drive DF0:</t>
+  </si>
+  <si>
+    <t>Floppy drive DF1:</t>
+  </si>
+  <si>
+    <t>Set configuration</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Start in Quickstart mode</t>
+  </si>
+  <si>
+    <t>Hardware emulato</t>
+  </si>
+  <si>
+    <t>Modello:</t>
+  </si>
+  <si>
+    <t>Configurazione:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compatibilità e potenza della CPU richiesta </t>
+  </si>
+  <si>
+    <t>Migliore compatibilità</t>
+  </si>
+  <si>
+    <t>Bassa compatibilità</t>
+  </si>
+  <si>
+    <t>Configurazione dell'host</t>
+  </si>
+  <si>
+    <t>Unità emulate</t>
+  </si>
+  <si>
+    <t>Unità floppy DF0:</t>
+  </si>
+  <si>
+    <t>Unità floppy DF1:</t>
+  </si>
+  <si>
+    <t>Selezionare il file immagine</t>
+  </si>
+  <si>
+    <t>Protezione da scrittura</t>
+  </si>
+  <si>
+    <t>Configurazione impostata</t>
+  </si>
+  <si>
+    <t>Modalità</t>
+  </si>
+  <si>
+    <t>Avvio in modalità Quickstart</t>
+  </si>
+  <si>
+    <t>Processing...</t>
+  </si>
+  <si>
+    <t>Elaborazione...</t>
+  </si>
+  <si>
+    <t>Enter text…</t>
+  </si>
+  <si>
+    <t>Inserire il testo...</t>
   </si>
 </sst>
 </file>
@@ -4028,10 +4253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F681"/>
+  <dimension ref="A1:F731"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A648" workbookViewId="0">
-      <selection activeCell="A682" sqref="A682"/>
+    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
+      <selection activeCell="B731" sqref="B731"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10445,7 +10670,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="641" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B641" t="s">
         <v>1139</v>
       </c>
@@ -10453,7 +10678,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="642" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B642" t="s">
         <v>1140</v>
       </c>
@@ -10461,7 +10686,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="643" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B643" t="s">
         <v>1141</v>
       </c>
@@ -10469,7 +10694,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="644" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B644" t="s">
         <v>1142</v>
       </c>
@@ -10477,7 +10702,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="645" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B645" t="s">
         <v>1143</v>
       </c>
@@ -10485,7 +10710,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="646" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B646" t="s">
         <v>1040</v>
       </c>
@@ -10493,7 +10718,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="647" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B647" t="s">
         <v>1144</v>
       </c>
@@ -10501,7 +10726,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="648" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B648" t="s">
         <v>1145</v>
       </c>
@@ -10509,7 +10734,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="649" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B649" t="s">
         <v>1148</v>
       </c>
@@ -10517,7 +10742,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="650" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B650" t="s">
         <v>1146</v>
       </c>
@@ -10525,7 +10750,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="651" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B651" t="s">
         <v>1147</v>
       </c>
@@ -10533,7 +10758,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="652" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>163</v>
       </c>
@@ -10543,11 +10768,8 @@
       <c r="C652" t="s">
         <v>1178</v>
       </c>
-      <c r="D652" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="653" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B653" t="s">
         <v>1163</v>
       </c>
@@ -10555,7 +10777,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="654" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B654" t="s">
         <v>926</v>
       </c>
@@ -10563,7 +10785,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="655" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B655" t="s">
         <v>1164</v>
       </c>
@@ -10571,7 +10793,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="656" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B656" t="s">
         <v>931</v>
       </c>
@@ -10781,11 +11003,423 @@
       <c r="A681">
         <v>184</v>
       </c>
+      <c r="B681" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C681" t="s">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B682" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C682" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B683" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C683" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B684" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C684" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B685" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C685" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="686" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B686" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C686" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B687" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C687" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B688" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C688" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="689" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B689" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C689" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B690" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C690" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B691" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C691" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B692" t="s">
+        <v>624</v>
+      </c>
+      <c r="C692" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B693" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C693" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="694" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B694" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C694" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="695" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B695" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C695" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="696" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B696" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C696" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="697" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B697" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C697" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="698" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B698" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C698" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="699" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B699" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C699" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="700" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B700" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C700" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="701" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B701" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C701" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="702" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B702" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C702" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="703" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A703">
+        <v>185</v>
+      </c>
+      <c r="B703" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C703" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D703" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="704" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B704" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C704" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="705" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B705" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C705" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="706" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B706" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C706" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="707" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B707" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C707" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="708" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B708" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C708" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="709" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B709" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C709" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="710" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B710" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C710" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="711" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B711" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C711" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="712" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B712" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C712" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="713" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B713" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C713" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="714" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B714" t="s">
+        <v>787</v>
+      </c>
+      <c r="C714" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="715" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B715" t="s">
+        <v>698</v>
+      </c>
+      <c r="C715" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="716" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B716" t="s">
+        <v>688</v>
+      </c>
+      <c r="C716" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="717" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B717" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C717" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="718" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B718" t="s">
+        <v>787</v>
+      </c>
+      <c r="C718" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="719" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B719" t="s">
+        <v>698</v>
+      </c>
+      <c r="C719" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="720" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B720" t="s">
+        <v>688</v>
+      </c>
+      <c r="C720" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B721" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C721" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B722" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C722" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B723" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C723" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A724">
+        <v>249</v>
+      </c>
+      <c r="B724" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B725" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A726">
+        <v>250</v>
+      </c>
+      <c r="B726" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C726" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B727" t="s">
+        <v>948</v>
+      </c>
+      <c r="C727" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A728">
+        <v>251</v>
+      </c>
+      <c r="B728" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C728" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B729" t="s">
+        <v>947</v>
+      </c>
+      <c r="C729" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B730" t="s">
+        <v>948</v>
+      </c>
+      <c r="C730" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A731">
+        <v>263</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D652" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D703" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mouse, Joystick and RTG translations added
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8E3666-B037-47D9-8EE3-950850393DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A43974-641D-45A2-BE6E-6FACDA71AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14235" yWindow="2205" windowWidth="23925" windowHeight="15315" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="8790" yWindow="7710" windowWidth="23925" windowHeight="11730" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="1276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1350">
   <si>
     <t>ID</t>
   </si>
@@ -3863,6 +3863,228 @@
   </si>
   <si>
     <t>Inserire il testo...</t>
+  </si>
+  <si>
+    <t>Mouse and Joystick settings</t>
+  </si>
+  <si>
+    <t>Port 1:</t>
+  </si>
+  <si>
+    <t>Port 2:</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap or test Port 1 configurarion.</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap or test Port 2 configuration.</t>
+  </si>
+  <si>
+    <t>Swap ports [] Swap ports 1 and 2.</t>
+  </si>
+  <si>
+    <t>Mouse/Joystick autoswitching [] Press button to automatically insert inactive input device in to joystick/mouse port</t>
+  </si>
+  <si>
+    <t>Emulated parallel port joystick adapter</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap or test Parallel port joystick port 1 configurarion.</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap or test Parallel port joystick port 2 configurarion.</t>
+  </si>
+  <si>
+    <t>Mouse extra settings</t>
+  </si>
+  <si>
+    <t>Mouse speed:</t>
+  </si>
+  <si>
+    <t>Install virtual mouse driver</t>
+  </si>
+  <si>
+    <t>Tablet.library emulation</t>
+  </si>
+  <si>
+    <t>Mouse untrap mode:</t>
+  </si>
+  <si>
+    <t>Magic Mouse cursor mode:</t>
+  </si>
+  <si>
+    <t>Tablet mode:</t>
+  </si>
+  <si>
+    <t>Impostazioni del mouse e del joystick</t>
+  </si>
+  <si>
+    <t>Porta 1:</t>
+  </si>
+  <si>
+    <t>Porta 2:</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap o test della configurazione della Porta 1.</t>
+  </si>
+  <si>
+    <t>Scambia le porte [] Scambia le porte 1 e 2.</t>
+  </si>
+  <si>
+    <t>Commutazione automatica mouse/Joystick [] Premere il pulsante per inserire automaticamente il dispositivo di ingresso inattivo nella porta joystick/mouse.</t>
+  </si>
+  <si>
+    <t>Adattatore joystick emulato per porta parallela</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap o test della configurazione della porta joystick 1 della porta parallela.</t>
+  </si>
+  <si>
+    <t>Remap / Test [] Remap o test della configurazione della porta joystick 2 della porta parallela.</t>
+  </si>
+  <si>
+    <t>Impostazioni extra del mouse</t>
+  </si>
+  <si>
+    <t>Velocità del mouse:</t>
+  </si>
+  <si>
+    <t>Installare il driver del mouse virtuale</t>
+  </si>
+  <si>
+    <t>Emulazione tablet.library</t>
+  </si>
+  <si>
+    <t>Modalità di rimozione del mouse:</t>
+  </si>
+  <si>
+    <t>Modalità cursore del mouse magico:</t>
+  </si>
+  <si>
+    <t>Modalità tablet:</t>
+  </si>
+  <si>
+    <t>Enter address...</t>
+  </si>
+  <si>
+    <t>Enter address</t>
+  </si>
+  <si>
+    <t>Inserire l'indirizzo...</t>
+  </si>
+  <si>
+    <t>Inserire l'indirizzo</t>
+  </si>
+  <si>
+    <t>RTG Graphics Card</t>
+  </si>
+  <si>
+    <t>Board:</t>
+  </si>
+  <si>
+    <t>VRAM size: [] Graphics card memory. Required for RTG (Picasso96) emulation.</t>
+  </si>
+  <si>
+    <t>Match host and RTG color depth if possible</t>
+  </si>
+  <si>
+    <t>Scale if smaller than display size setting</t>
+  </si>
+  <si>
+    <t>Always scale in windowed mode</t>
+  </si>
+  <si>
+    <t>Always center</t>
+  </si>
+  <si>
+    <t>Hardware vertical blank interrupt</t>
+  </si>
+  <si>
+    <t>Multithreaded</t>
+  </si>
+  <si>
+    <t>Hardware sprite emulation</t>
+  </si>
+  <si>
+    <t>Color modes:</t>
+  </si>
+  <si>
+    <t>Refresh rate:</t>
+  </si>
+  <si>
+    <t>Buffer mode:</t>
+  </si>
+  <si>
+    <t>Aspect ratio:</t>
+  </si>
+  <si>
+    <t>Scheda grafica RTG</t>
+  </si>
+  <si>
+    <t>Consiglio:</t>
+  </si>
+  <si>
+    <t>Dimensione VRAM: [] Memoria della scheda grafica. Richiesto per l'emulazione RTG (Picasso96).</t>
+  </si>
+  <si>
+    <t>Se possibile, far coincidere la profondità di colore dell'host e dell'RTG</t>
+  </si>
+  <si>
+    <t>Scala se inferiore alle dimensioni del display impostate</t>
+  </si>
+  <si>
+    <t>Scala sempre in modalità a finestre</t>
+  </si>
+  <si>
+    <t>Sempre al centro</t>
+  </si>
+  <si>
+    <t>Interruzione hardware del vuoto verticale</t>
+  </si>
+  <si>
+    <t>Emulazione hardware degli sprite</t>
+  </si>
+  <si>
+    <t>Modalità di colore:</t>
+  </si>
+  <si>
+    <t>Frequenza di aggiornamento:</t>
+  </si>
+  <si>
+    <t>Modalità buffer:</t>
+  </si>
+  <si>
+    <t>Rapporto d'aspetto:</t>
+  </si>
+  <si>
+    <t>Input Remap</t>
+  </si>
+  <si>
+    <t>Rimodulazione degli ingressi</t>
+  </si>
+  <si>
+    <t>Scanning ROM image files...</t>
+  </si>
+  <si>
+    <t>Scansione dei file immagine ROM...</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Libero</t>
+  </si>
+  <si>
+    <t>CD Settings</t>
+  </si>
+  <si>
+    <t>Add CD Drive</t>
+  </si>
+  <si>
+    <t>Impostazioni del CD</t>
+  </si>
+  <si>
+    <t>Aggiungere l'unità CD</t>
   </si>
 </sst>
 </file>
@@ -4253,10 +4475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F731"/>
+  <dimension ref="A1:F783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
-      <selection activeCell="B731" sqref="B731"/>
+    <sheetView tabSelected="1" topLeftCell="A761" workbookViewId="0">
+      <selection activeCell="A784" sqref="A784"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11066,7 +11288,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="689" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B689" t="s">
         <v>1209</v>
       </c>
@@ -11074,7 +11296,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="690" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B690" t="s">
         <v>1210</v>
       </c>
@@ -11082,7 +11304,7 @@
         <v>1231</v>
       </c>
     </row>
-    <row r="691" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B691" t="s">
         <v>1211</v>
       </c>
@@ -11090,7 +11312,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="692" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B692" t="s">
         <v>624</v>
       </c>
@@ -11098,7 +11320,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="693" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B693" t="s">
         <v>1212</v>
       </c>
@@ -11106,7 +11328,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="694" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B694" t="s">
         <v>1213</v>
       </c>
@@ -11114,7 +11336,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="695" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B695" t="s">
         <v>1214</v>
       </c>
@@ -11122,7 +11344,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="696" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B696" t="s">
         <v>1215</v>
       </c>
@@ -11130,7 +11352,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="697" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B697" t="s">
         <v>1216</v>
       </c>
@@ -11138,7 +11360,7 @@
         <v>1238</v>
       </c>
     </row>
-    <row r="698" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B698" t="s">
         <v>1217</v>
       </c>
@@ -11146,7 +11368,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="699" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B699" t="s">
         <v>1218</v>
       </c>
@@ -11154,7 +11376,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="700" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B700" t="s">
         <v>1219</v>
       </c>
@@ -11162,7 +11384,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="701" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="701" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B701" t="s">
         <v>1220</v>
       </c>
@@ -11170,7 +11392,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="702" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B702" t="s">
         <v>1221</v>
       </c>
@@ -11178,7 +11400,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="703" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="703" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A703">
         <v>185</v>
       </c>
@@ -11188,11 +11410,8 @@
       <c r="C703" t="s">
         <v>1257</v>
       </c>
-      <c r="D703" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="704" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="704" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B704" t="s">
         <v>1245</v>
       </c>
@@ -11328,7 +11547,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B721" t="s">
         <v>1254</v>
       </c>
@@ -11336,7 +11555,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B722" t="s">
         <v>1255</v>
       </c>
@@ -11344,7 +11563,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B723" t="s">
         <v>1256</v>
       </c>
@@ -11352,7 +11571,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A724">
         <v>249</v>
       </c>
@@ -11360,12 +11579,12 @@
         <v>773</v>
       </c>
     </row>
-    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B725" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A726">
         <v>250</v>
       </c>
@@ -11376,7 +11595,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B727" t="s">
         <v>948</v>
       </c>
@@ -11384,7 +11603,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A728">
         <v>251</v>
       </c>
@@ -11395,7 +11614,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B729" t="s">
         <v>947</v>
       </c>
@@ -11403,7 +11622,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B730" t="s">
         <v>948</v>
       </c>
@@ -11411,15 +11630,443 @@
         <v>970</v>
       </c>
     </row>
-    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A731">
         <v>263</v>
+      </c>
+      <c r="B731" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C731" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D731" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B732" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C732" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B733" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C733" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B734" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C734" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B735" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C735" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B736" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C736" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="737" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B737" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C737" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="738" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B738" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C738" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="739" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B739" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C739" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="740" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B740" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C740" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="741" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B741" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C741" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="742" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B742" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C742" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="743" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B743" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C743" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="744" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B744" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C744" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="745" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B745" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C745" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="746" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B746" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C746" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="747" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B747" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C747" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="748" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A748">
+        <v>335</v>
+      </c>
+      <c r="B748" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C748" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="749" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B749" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C749" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="750" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B750" t="s">
+        <v>947</v>
+      </c>
+      <c r="C750" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="751" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B751" t="s">
+        <v>948</v>
+      </c>
+      <c r="C751" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="752" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A752">
+        <v>351</v>
+      </c>
+      <c r="B752" t="s">
+        <v>1313</v>
+      </c>
+      <c r="C752" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="753" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B753" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C753" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="754" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B754" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C754" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="755" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B755" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C755" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="756" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B756" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C756" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B757" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C757" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="758" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B758" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C758" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="759" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B759" t="s">
+        <v>1319</v>
+      </c>
+      <c r="C759" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="760" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B760" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C760" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="761" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B761" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C761" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="762" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B762" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C762" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="763" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B763" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C763" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="764" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B764" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C764" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="765" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B765" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C765" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="766" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B766" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C766" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="767" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A767">
+        <v>354</v>
+      </c>
+      <c r="B767" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C767" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="768" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B768" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="769" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A769">
+        <v>355</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C769" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="770" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B770" t="s">
+        <v>947</v>
+      </c>
+      <c r="C770" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="771" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B771" t="s">
+        <v>948</v>
+      </c>
+      <c r="C771" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="772" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A772">
+        <v>386</v>
+      </c>
+      <c r="B772" t="s">
+        <v>778</v>
+      </c>
+      <c r="C772" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="773" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B773" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="774" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B774" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="775" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B775" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C775" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="776" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B776" t="s">
+        <v>947</v>
+      </c>
+      <c r="C776" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="777" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B777" t="s">
+        <v>948</v>
+      </c>
+      <c r="C777" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="778" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A778">
+        <v>387</v>
+      </c>
+      <c r="B778" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C778" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="779" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B779" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="780" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B780" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="781" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B781" t="s">
+        <v>935</v>
+      </c>
+      <c r="C781" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="782" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B782" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C782" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="783" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B783" t="s">
+        <v>948</v>
+      </c>
+      <c r="C783" t="s">
+        <v>970</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D703" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D731" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Last set of translations
</commit_message>
<xml_diff>
--- a/Italian translation for Winuae.xlsx
+++ b/Italian translation for Winuae.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\WinUAE\Translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A43974-641D-45A2-BE6E-6FACDA71AE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D4FA5-DB16-4609-9D77-37C731762DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8790" yWindow="7710" windowWidth="23925" windowHeight="11730" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
+    <workbookView xWindow="12780" yWindow="4455" windowWidth="26025" windowHeight="16935" xr2:uid="{3D11DA74-8E24-4E5F-8FCA-E4D9010E6A34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="1350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="1435">
   <si>
     <t>ID</t>
   </si>
@@ -4085,13 +4085,268 @@
   </si>
   <si>
     <t>Aggiungere l'unità CD</t>
+  </si>
+  <si>
+    <t>Tape Drive Settings</t>
+  </si>
+  <si>
+    <t>Add Tape Drive</t>
+  </si>
+  <si>
+    <t>Impostazioni dell'unità a nastro</t>
+  </si>
+  <si>
+    <t>Aggiungi unità a nastro</t>
+  </si>
+  <si>
+    <t>Configuration error log</t>
+  </si>
+  <si>
+    <t>Clear log</t>
+  </si>
+  <si>
+    <t>Registro degli errori di configurazione</t>
+  </si>
+  <si>
+    <t>Cancella registro</t>
+  </si>
+  <si>
+    <t>Disk image information</t>
+  </si>
+  <si>
+    <t>Informazioni sull'immagine del disco</t>
+  </si>
+  <si>
+    <t>Risparmiare</t>
+  </si>
+  <si>
+    <t>Expansion Board Settings</t>
+  </si>
+  <si>
+    <t>24-bit DMA</t>
+  </si>
+  <si>
+    <t>Controller ID:</t>
+  </si>
+  <si>
+    <t>Autoboot disabled</t>
+  </si>
+  <si>
+    <t>PCMCIA inserted</t>
+  </si>
+  <si>
+    <t>Accelerator Board Settings</t>
+  </si>
+  <si>
+    <t>Accelerator board ROM file:</t>
+  </si>
+  <si>
+    <t>Accelerator board memory:</t>
+  </si>
+  <si>
+    <t>Miscellaneous Expansions</t>
+  </si>
+  <si>
+    <t>bsdsocket.library [] bsdsocket network library emulation.</t>
+  </si>
+  <si>
+    <t>uaescsi.device</t>
+  </si>
+  <si>
+    <t>uaenet.device [] Sana 2 compatible network device emulation.</t>
+  </si>
+  <si>
+    <t>CD32 Full Motion Video cartridge</t>
+  </si>
+  <si>
+    <t>Impostazioni della scheda di espansione</t>
+  </si>
+  <si>
+    <t>DMA a 24 bit</t>
+  </si>
+  <si>
+    <t>ID controllore:</t>
+  </si>
+  <si>
+    <t>Autoboot disabilitato</t>
+  </si>
+  <si>
+    <t>PCMCIA inserito</t>
+  </si>
+  <si>
+    <t>Impostazioni della scheda acceleratore</t>
+  </si>
+  <si>
+    <t>File ROM della scheda acceleratore:</t>
+  </si>
+  <si>
+    <t>Memoria della scheda acceleratore:</t>
+  </si>
+  <si>
+    <t>Espansioni varie</t>
+  </si>
+  <si>
+    <t>bsdsocket.library [] emulazione della libreria di rete bsdsocket.</t>
+  </si>
+  <si>
+    <t>uaenet.device [] Emulazione del dispositivo di rete compatibile con Sana 2.</t>
+  </si>
+  <si>
+    <t>Cartuccia video full motion CD32</t>
+  </si>
+  <si>
+    <t>Custom board order</t>
+  </si>
+  <si>
+    <t>Move up</t>
+  </si>
+  <si>
+    <t>Move down</t>
+  </si>
+  <si>
+    <t>Ordine di schede personalizzate</t>
+  </si>
+  <si>
+    <t>Salire</t>
+  </si>
+  <si>
+    <t>Scendere</t>
+  </si>
+  <si>
+    <t>CHS Geometry</t>
+  </si>
+  <si>
+    <t>Heads:</t>
+  </si>
+  <si>
+    <t>Geometria CHS</t>
+  </si>
+  <si>
+    <t>Teste:</t>
+  </si>
+  <si>
+    <t>WinUAE Properties</t>
+  </si>
+  <si>
+    <t>Proprietà di WinUAE</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Eject all drives</t>
+  </si>
+  <si>
+    <t>DF0: - DF3:</t>
+  </si>
+  <si>
+    <t>CD drives</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Quit Winuae</t>
+  </si>
+  <si>
+    <t>Configurazione</t>
+  </si>
+  <si>
+    <t>Espulsione di tutte le unità</t>
+  </si>
+  <si>
+    <t>Unità CD</t>
+  </si>
+  <si>
+    <t>Aiuto</t>
+  </si>
+  <si>
+    <t>Abbandono di Winuae</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Disassembly</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Copy line</t>
+  </si>
+  <si>
+    <t>Copy all</t>
+  </si>
+  <si>
+    <t>Set top address</t>
+  </si>
+  <si>
+    <t>Set to A0 to A7</t>
+  </si>
+  <si>
+    <t>Breakpoints</t>
+  </si>
+  <si>
+    <t>Toggle breakpoint</t>
+  </si>
+  <si>
+    <t>Clear all breakpoints</t>
+  </si>
+  <si>
+    <t>Set to PC</t>
+  </si>
+  <si>
+    <t>Inattivo</t>
+  </si>
+  <si>
+    <t>Copia</t>
+  </si>
+  <si>
+    <t>Copia della linea</t>
+  </si>
+  <si>
+    <t>Copiare tutti</t>
+  </si>
+  <si>
+    <t>Memoria</t>
+  </si>
+  <si>
+    <t>Indirizzo del set top</t>
+  </si>
+  <si>
+    <t>Impostato su A0</t>
+  </si>
+  <si>
+    <t>Smontaggio</t>
+  </si>
+  <si>
+    <t>Punti di rottura</t>
+  </si>
+  <si>
+    <t>Attiva il punto di interruzione</t>
+  </si>
+  <si>
+    <t>Cancella tutti i punti di interruzione</t>
+  </si>
+  <si>
+    <t>Impostare su PC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4128,6 +4383,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4150,7 +4413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4160,6 +4423,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4475,10 +4739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF4BD0E4-D4EF-4947-A2DD-A8FCDBFF80BF}">
-  <dimension ref="A1:F783"/>
+  <dimension ref="A1:F861"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A761" workbookViewId="0">
-      <selection activeCell="A784" sqref="A784"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11547,7 +11811,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="721" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B721" t="s">
         <v>1254</v>
       </c>
@@ -11555,7 +11819,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="722" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B722" t="s">
         <v>1255</v>
       </c>
@@ -11563,7 +11827,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="723" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B723" t="s">
         <v>1256</v>
       </c>
@@ -11571,7 +11835,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="724" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A724">
         <v>249</v>
       </c>
@@ -11579,12 +11843,12 @@
         <v>773</v>
       </c>
     </row>
-    <row r="725" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B725" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="726" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A726">
         <v>250</v>
       </c>
@@ -11595,7 +11859,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="727" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B727" t="s">
         <v>948</v>
       </c>
@@ -11603,7 +11867,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="728" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A728">
         <v>251</v>
       </c>
@@ -11614,7 +11878,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="729" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B729" t="s">
         <v>947</v>
       </c>
@@ -11622,7 +11886,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="730" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B730" t="s">
         <v>948</v>
       </c>
@@ -11630,7 +11894,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="731" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A731">
         <v>263</v>
       </c>
@@ -11640,11 +11904,8 @@
       <c r="C731" t="s">
         <v>1293</v>
       </c>
-      <c r="D731" s="5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="732" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="732" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B732" t="s">
         <v>1277</v>
       </c>
@@ -11652,7 +11913,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="733" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="733" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B733" t="s">
         <v>1279</v>
       </c>
@@ -11660,7 +11921,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="734" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B734" t="s">
         <v>1278</v>
       </c>
@@ -11668,7 +11929,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="735" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="735" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B735" t="s">
         <v>1280</v>
       </c>
@@ -11676,7 +11937,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="736" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="736" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B736" t="s">
         <v>1281</v>
       </c>
@@ -12063,10 +12324,638 @@
         <v>970</v>
       </c>
     </row>
+    <row r="784" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A784">
+        <v>388</v>
+      </c>
+      <c r="B784" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C784" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="785" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B785" t="s">
+        <v>924</v>
+      </c>
+      <c r="C785" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="786" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B786" t="s">
+        <v>973</v>
+      </c>
+      <c r="C786" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="787" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B787" t="s">
+        <v>974</v>
+      </c>
+      <c r="C787" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="788" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B788" t="s">
+        <v>688</v>
+      </c>
+      <c r="C788" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="789" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B789" t="s">
+        <v>935</v>
+      </c>
+      <c r="C789" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="790" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B790" t="s">
+        <v>931</v>
+      </c>
+      <c r="C790" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="791" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B791" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C791" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="792" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B792" t="s">
+        <v>948</v>
+      </c>
+      <c r="C792" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="793" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A793">
+        <v>389</v>
+      </c>
+      <c r="B793" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C793" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="794" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B794" t="s">
+        <v>947</v>
+      </c>
+      <c r="C794" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="795" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B795" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C795" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="796" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A796">
+        <v>390</v>
+      </c>
+      <c r="B796" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C796" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="797" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B797" t="s">
+        <v>947</v>
+      </c>
+      <c r="C797" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="798" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B798" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C798" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="799" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A799">
+        <v>398</v>
+      </c>
+      <c r="B799" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C799" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D799" s="5" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="800" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B800" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C800" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B801" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C801" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="802" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B802" t="s">
+        <v>819</v>
+      </c>
+      <c r="C802" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="803" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B803" t="s">
+        <v>1364</v>
+      </c>
+      <c r="C803" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="804" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B804" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C804" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B805" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C805" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B806" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C806" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B807" t="s">
+        <v>1368</v>
+      </c>
+      <c r="C807" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="808" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B808" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C808" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="809" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B809" t="s">
+        <v>1370</v>
+      </c>
+      <c r="C809" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="810" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B810" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C810" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="811" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B811" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C811" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="812" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B812" t="s">
+        <v>1373</v>
+      </c>
+      <c r="C812" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="813" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A813">
+        <v>399</v>
+      </c>
+      <c r="B813" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="814" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B814" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="815" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B815" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C815" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="816" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B816" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C816" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="817" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B817" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C817" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="818" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A818">
+        <v>400</v>
+      </c>
+      <c r="B818" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C818" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="819" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B819" t="s">
+        <v>939</v>
+      </c>
+      <c r="C819" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B820" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C820" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="821" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B821" t="s">
+        <v>938</v>
+      </c>
+      <c r="C821" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="822" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B822" t="s">
+        <v>947</v>
+      </c>
+      <c r="C822" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="823" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B823" t="s">
+        <v>948</v>
+      </c>
+      <c r="C823" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="824" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A824">
+        <v>51</v>
+      </c>
+      <c r="B824" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C824" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="825" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B825" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="826" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B826" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="827" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B827" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="829" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A829" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="830" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A830">
+        <v>186</v>
+      </c>
+      <c r="B830" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C830" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="831" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B831" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C831" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="832" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B832" t="s">
+        <v>9</v>
+      </c>
+      <c r="C832" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="833" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B833" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C833" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="834" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B834" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C834" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="835" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B835" t="s">
+        <v>1402</v>
+      </c>
+      <c r="C835" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="836" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B836" t="s">
+        <v>688</v>
+      </c>
+      <c r="C836" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="837" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B837" t="s">
+        <v>310</v>
+      </c>
+      <c r="C837" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="838" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B838" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C838" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="839" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B839" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C839" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="840" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B840" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C840" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="841" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A841">
+        <v>334</v>
+      </c>
+      <c r="B841" s="7" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C841" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="842" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B842" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C842" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="843" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B843" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C843" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="844" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B844" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C844" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="845" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B845" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C845" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="846" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B846" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C846" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="847" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B847" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C847" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="848" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B848" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C848" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="849" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B849" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C849" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="850" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B850" t="s">
+        <v>1418</v>
+      </c>
+      <c r="C850" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="851" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B851" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C851" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="852" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B852" s="7" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C852" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="853" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B853" t="s">
+        <v>1414</v>
+      </c>
+      <c r="C853" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="854" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B854" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C854" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="855" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B855" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C855" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="856" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B856" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C856" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="857" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B857" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C857" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="858" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B858" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C858" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="859" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B859" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C859" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="860" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B860" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C860" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="861" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B861" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C861" t="s">
+        <v>1312</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F1" r:id="rId1" display="https://www.deepl.com/translator" xr:uid="{6E39C4FC-6A4D-40E9-929C-2FDA285A8DD0}"/>
-    <hyperlink ref="D731" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
+    <hyperlink ref="D799" r:id="rId2" display="https://www.deepl.com/translator" xr:uid="{F28C17BE-F547-4262-815D-996477ADBE2F}"/>
     <hyperlink ref="E314" r:id="rId3" xr:uid="{E36EE6F4-CD00-463F-A98F-BAAC015A3A1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>